<commit_message>
Modification to airfare computation and elasticity fro marginal cost pricing
</commit_message>
<xml_diff>
--- a/aeromaps/resources/cost_data/IATA_cost_data.xlsx
+++ b/aeromaps/resources/cost_data/IATA_cost_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.salgas.ISAE-SUPAERO\PycharmProjects\AeroMAPS\aeromaps\resources\cost_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A206191-78B5-45BB-B5AC-12A1BC3DB647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080630B8-2D84-4782-89E5-F677E683ADE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{21AF616A-B21B-4352-988D-7E50970EE7EE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{21AF616A-B21B-4352-988D-7E50970EE7EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
   <si>
     <t>Station expenses</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>Total 'Pax' Nprof (B USD)</t>
+  </si>
+  <si>
+    <t>Initial AVG price</t>
   </si>
 </sst>
 </file>
@@ -856,25 +859,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F797DD12-7B4A-4D77-BF80-431EC5125AE0}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="121.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="121.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -894,7 +897,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -912,7 +915,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
@@ -930,7 +933,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
@@ -948,7 +951,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
@@ -966,7 +969,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
@@ -984,7 +987,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
@@ -1002,7 +1005,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
@@ -1020,7 +1023,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
@@ -1038,7 +1041,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>8</v>
       </c>
@@ -1056,7 +1059,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>9</v>
       </c>
@@ -1074,7 +1077,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>10</v>
       </c>
@@ -1092,7 +1095,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>11</v>
       </c>
@@ -1110,8 +1113,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="23" t="s">
         <v>43</v>
       </c>
@@ -1120,7 +1123,7 @@
       <c r="E19" s="24"/>
       <c r="F19" s="25"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="17" t="s">
         <v>35</v>
       </c>
@@ -1135,7 +1138,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="17"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
@@ -1146,7 +1149,7 @@
         <v>85.8</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="19" t="s">
         <v>20</v>
       </c>
@@ -1169,7 +1172,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="17"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -1186,7 +1189,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="17" t="s">
         <v>37</v>
       </c>
@@ -1209,7 +1212,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="17" t="s">
         <v>38</v>
       </c>
@@ -1231,7 +1234,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="17" t="s">
         <v>28</v>
       </c>
@@ -1247,7 +1250,7 @@
         <v>22.651199999999999</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="17" t="s">
         <v>30</v>
       </c>
@@ -1258,7 +1261,7 @@
       <c r="E27" s="15"/>
       <c r="F27" s="18"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="17" t="s">
         <v>29</v>
       </c>
@@ -1270,14 +1273,14 @@
       <c r="E28" s="15"/>
       <c r="F28" s="18"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="17"/>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
       <c r="F29" s="18"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="17" t="s">
         <v>31</v>
       </c>
@@ -1294,7 +1297,7 @@
         <v>6.8516071065989836E-2</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" s="17" t="s">
         <v>32</v>
       </c>
@@ -1311,7 +1314,7 @@
         <v>3.5320934010152276E-3</v>
       </c>
     </row>
-    <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="20" t="s">
         <v>44</v>
       </c>
@@ -1323,10 +1326,19 @@
       <c r="E32" s="21"/>
       <c r="F32" s="22"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E34">
         <f>F30-C32</f>
         <v>3.5157411167513197E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E37" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37">
+        <f>F22/C26</f>
+        <v>8.2949238578680196E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All core noteboks outputs checked and validated with TP
</commit_message>
<xml_diff>
--- a/aeromaps/resources/cost_data/IATA_cost_data.xlsx
+++ b/aeromaps/resources/cost_data/IATA_cost_data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.salgas.ISAE-SUPAERO\PycharmProjects\AeroMAPS\aeromaps\resources\cost_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a.salgas/PycharmProjects/AeroMAPS/aeromaps/resources/cost_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A206191-78B5-45BB-B5AC-12A1BC3DB647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE34E624-068E-654C-A194-541A0145F15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{21AF616A-B21B-4352-988D-7E50970EE7EE}"/>
+    <workbookView xWindow="29560" yWindow="-8760" windowWidth="38080" windowHeight="20780" activeTab="1" xr2:uid="{21AF616A-B21B-4352-988D-7E50970EE7EE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Recap 2019" sheetId="1" r:id="rId1"/>
+    <sheet name="Exploration" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
   <si>
     <t>Station expenses</t>
   </si>
@@ -180,13 +181,112 @@
   </si>
   <si>
     <t>Total 'Pax' Nprof (B USD)</t>
+  </si>
+  <si>
+    <t>Initial AVG price</t>
+  </si>
+  <si>
+    <t>REVENUES, $ billion</t>
+  </si>
+  <si>
+    <t>Passenger, $ billion</t>
+  </si>
+  <si>
+    <t>Cargo, $ billion</t>
+  </si>
+  <si>
+    <t>Scheduled passenger numbers, millions</t>
+  </si>
+  <si>
+    <t>Freight tonnes, millions</t>
+  </si>
+  <si>
+    <t>World economic growth, %</t>
+  </si>
+  <si>
+    <t>EXPENSES, $ billion</t>
+  </si>
+  <si>
+    <t>Fuel, $ billion</t>
+  </si>
+  <si>
+    <t>Jet kerosene price, $/b</t>
+  </si>
+  <si>
+    <t>Non-fuel, $ billion</t>
+  </si>
+  <si>
+    <t>OPERATING PROFIT, $ billion</t>
+  </si>
+  <si>
+    <t>NET PROFIT, $ billion</t>
+  </si>
+  <si>
+    <t>REFS</t>
+  </si>
+  <si>
+    <t>https://www.iata.org/en/iata-repository/publications/economic-reports/airline-industry-economic-performance---2018-mid-year---table/</t>
+  </si>
+  <si>
+    <t>https://www.iata.org/en/iata-repository/pressroom/fact-sheets/industry-statistics</t>
+  </si>
+  <si>
+    <t>All but RPK -until 2019</t>
+  </si>
+  <si>
+    <t>All but RPK from 2019</t>
+  </si>
+  <si>
+    <t>RPK 2000-2018</t>
+  </si>
+  <si>
+    <t>https://www.statista.com/statistics/1261233/air-revenue-passenger-kilometers-worldwide/</t>
+  </si>
+  <si>
+    <t>RPK from 2019</t>
+  </si>
+  <si>
+    <t>PLF, %</t>
+  </si>
+  <si>
+    <t>Estimated</t>
+  </si>
+  <si>
+    <t>Forecast</t>
+  </si>
+  <si>
+    <t>% gross margin</t>
+  </si>
+  <si>
+    <t>% net margin</t>
+  </si>
+  <si>
+    <t>RPKs, billion</t>
+  </si>
+  <si>
+    <t>Passenger + anx (share), $ billion</t>
+  </si>
+  <si>
+    <t>ASKs, billion</t>
+  </si>
+  <si>
+    <t>Avg price, $/RPK</t>
+  </si>
+  <si>
+    <t>Avg price (incl. anx), $/RPK</t>
+  </si>
+  <si>
+    <t>Passenger + anx (share) expenses, $ billion</t>
+  </si>
+  <si>
+    <t>Avg cost, $/RPK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,8 +300,16 @@
       <name val="Bahnschrift"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,8 +322,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -438,11 +552,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -454,10 +654,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -465,7 +664,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -478,6 +676,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -502,6 +713,1204 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Margin</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> vs year</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Net Margin</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Exploration!$B$1:$W$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2025</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Exploration!$B$23:$W$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>-1.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-35.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-7.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D491-DB43-83FE-7103F452FE03}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Gross Margin</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Exploration!$B$1:$W$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2025</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Exploration!$B$21:$W$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-28.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-8.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D491-DB43-83FE-7103F452FE03}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1853569760"/>
+        <c:axId val="1853637232"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1853569760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1853637232"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1853637232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1853569760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -559,10 +1968,51 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2054864</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>78740</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>693419</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>78740</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFAE85BE-BB3A-2C2B-BB92-225276786E4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -600,7 +2050,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -706,7 +2156,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -848,7 +2298,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -856,25 +2306,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F797DD12-7B4A-4D77-BF80-431EC5125AE0}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="121.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="121.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -890,275 +2340,275 @@
       <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="9">
         <v>7.59745287438564</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3">
         <f>$C$22*B3/100</f>
         <v>51.822985801471887</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="9">
         <v>6.4911056174773396</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4">
         <f t="shared" ref="C4:C14" si="0">$C$22*B4/100</f>
         <v>44.27648052737468</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="9">
         <v>6.53611549051125</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5">
         <f t="shared" si="0"/>
         <v>44.583497372326292</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="9">
         <v>9.3826505362653894</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6">
         <f t="shared" si="0"/>
         <v>63.999997572919845</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="9">
         <v>7.5125641017892502</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7">
         <f t="shared" si="0"/>
         <v>51.243950994714659</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="9">
         <v>6.4836930421353101</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8">
         <f t="shared" si="0"/>
         <v>44.225918609709161</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" t="s">
         <v>25</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="9">
         <v>2.40748167477265</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9">
         <f t="shared" si="0"/>
         <v>16.421673251791724</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="9">
         <v>23.6905499177571</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10">
         <f t="shared" si="0"/>
         <v>161.59561004401294</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="9">
         <v>9.1315797805765406</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11">
         <f t="shared" si="0"/>
         <v>62.287418841290645</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="9">
         <v>6.0887638119529699</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12">
         <f t="shared" si="0"/>
         <v>41.532066837712399</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="9">
         <v>6.0766314104670398</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13">
         <f t="shared" si="0"/>
         <v>41.449310513936723</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="11">
         <v>8.60141174190945</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="12">
         <f t="shared" si="0"/>
         <v>58.67108963273855</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="23" t="s">
+    <row r="18" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="25"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="17" t="s">
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="34"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="13">
         <v>795</v>
       </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15" t="s">
+      <c r="D20" s="13"/>
+      <c r="E20" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="16">
         <v>838</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="17"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="16" t="s">
+    <row r="21" spans="2:10" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="15"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="16">
         <v>85.8</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="19" t="s">
+    <row r="22" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B22" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="13">
         <f>C20*F21/100</f>
         <v>682.11</v>
       </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15" t="s">
+      <c r="D22" s="13"/>
+      <c r="E22" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="16">
         <f>F20*F21/100</f>
         <v>719.00399999999991</v>
       </c>
@@ -1169,14 +2619,14 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="17"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15" t="s">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B23" s="15"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="18">
+      <c r="F23" s="16">
         <v>43.2</v>
       </c>
       <c r="I23" s="3" t="s">
@@ -1186,19 +2636,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="17" t="s">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B24" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="13">
         <f>SUMIF(D3:D14,"=yes",C3:C14)</f>
         <v>387.83576966953484</v>
       </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15" t="s">
+      <c r="D24" s="13"/>
+      <c r="E24" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="16">
         <f>F23*F21/100</f>
         <v>37.065599999999996</v>
       </c>
@@ -1209,19 +2659,19 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="17" t="s">
+    <row r="25" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="13">
         <f>SUMIF(E3:E14,"=yes",C3:C14)</f>
         <v>294.27423033046466</v>
       </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15" t="s">
+      <c r="D25" s="13"/>
+      <c r="E25" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="18">
+      <c r="F25" s="16">
         <v>26.4</v>
       </c>
       <c r="I25" s="5" t="s">
@@ -1231,102 +2681,117 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="17" t="s">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B26" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="13">
         <v>8668</v>
       </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15" t="s">
+      <c r="D26" s="13"/>
+      <c r="E26" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F26" s="18">
+      <c r="F26" s="16">
         <f>F25*F21/100</f>
         <v>22.651199999999999</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="17" t="s">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B27" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="13">
         <v>82.6</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="18"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="17" t="s">
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="16"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B28" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="13">
         <f>C26/(C27/100)</f>
         <v>10493.946731234868</v>
       </c>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="18"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="17"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="18"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="17" t="s">
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="16"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B29" s="15"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="16"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B30" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="13">
         <f>C24/C28</f>
         <v>3.6958046348296691E-2</v>
       </c>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15" t="s">
+      <c r="D30" s="13"/>
+      <c r="E30" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F30" s="18">
+      <c r="F30" s="16">
         <f>F22/C28</f>
         <v>6.8516071065989836E-2</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="17" t="s">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B31" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="13">
         <f>C25/C28</f>
         <v>2.8042283600941829E-2</v>
       </c>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15" t="s">
+      <c r="D31" s="13"/>
+      <c r="E31" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="18">
+      <c r="F31" s="16">
         <f>F24/C28</f>
         <v>3.5320934010152276E-3</v>
       </c>
     </row>
-    <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="20" t="s">
+    <row r="32" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="21">
+      <c r="C32" s="19">
         <f>C30+C31</f>
         <v>6.5000329949238517E-2</v>
       </c>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="22"/>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="20"/>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E34">
         <f>F30-C32</f>
         <v>3.5157411167513197E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E37" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37">
+        <f>F22/C26</f>
+        <v>8.2949238578680196E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <f>C32/C27*100</f>
+        <v>7.8692893401015152E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1337,4 +2802,1812 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0427CF9A-7727-6944-B3E2-D626E1863BCC}">
+  <dimension ref="A1:W61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A30" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" s="27"/>
+      <c r="B1" s="21">
+        <v>2004</v>
+      </c>
+      <c r="C1" s="21">
+        <v>2005</v>
+      </c>
+      <c r="D1" s="21">
+        <v>2006</v>
+      </c>
+      <c r="E1" s="21">
+        <v>2007</v>
+      </c>
+      <c r="F1" s="21">
+        <v>2008</v>
+      </c>
+      <c r="G1" s="21">
+        <v>2009</v>
+      </c>
+      <c r="H1" s="21">
+        <v>2010</v>
+      </c>
+      <c r="I1" s="21">
+        <v>2011</v>
+      </c>
+      <c r="J1" s="21">
+        <v>2012</v>
+      </c>
+      <c r="K1" s="21">
+        <v>2013</v>
+      </c>
+      <c r="L1" s="21">
+        <v>2014</v>
+      </c>
+      <c r="M1" s="21">
+        <v>2015</v>
+      </c>
+      <c r="N1" s="21">
+        <v>2016</v>
+      </c>
+      <c r="O1" s="21">
+        <v>2017</v>
+      </c>
+      <c r="P1" s="21">
+        <v>2018</v>
+      </c>
+      <c r="Q1" s="21">
+        <v>2019</v>
+      </c>
+      <c r="R1" s="21">
+        <v>2020</v>
+      </c>
+      <c r="S1" s="21">
+        <v>2021</v>
+      </c>
+      <c r="T1" s="21">
+        <v>2022</v>
+      </c>
+      <c r="U1" s="21">
+        <v>2023</v>
+      </c>
+      <c r="V1" s="21">
+        <v>2024</v>
+      </c>
+      <c r="W1" s="22">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2">
+        <v>379</v>
+      </c>
+      <c r="C2">
+        <v>413</v>
+      </c>
+      <c r="D2">
+        <v>465</v>
+      </c>
+      <c r="E2">
+        <v>510</v>
+      </c>
+      <c r="F2">
+        <v>570</v>
+      </c>
+      <c r="G2">
+        <v>476</v>
+      </c>
+      <c r="H2">
+        <v>564</v>
+      </c>
+      <c r="I2">
+        <v>642</v>
+      </c>
+      <c r="J2">
+        <v>706</v>
+      </c>
+      <c r="K2">
+        <v>720</v>
+      </c>
+      <c r="L2">
+        <v>767</v>
+      </c>
+      <c r="M2">
+        <v>721</v>
+      </c>
+      <c r="N2">
+        <v>709</v>
+      </c>
+      <c r="O2">
+        <v>754</v>
+      </c>
+      <c r="P2">
+        <v>812</v>
+      </c>
+      <c r="Q2">
+        <v>838</v>
+      </c>
+      <c r="R2">
+        <v>384</v>
+      </c>
+      <c r="S2">
+        <v>513</v>
+      </c>
+      <c r="T2">
+        <v>738</v>
+      </c>
+      <c r="U2">
+        <v>909</v>
+      </c>
+      <c r="V2">
+        <v>966</v>
+      </c>
+      <c r="W2" s="23">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>294</v>
+      </c>
+      <c r="C3">
+        <v>323</v>
+      </c>
+      <c r="D3">
+        <v>365</v>
+      </c>
+      <c r="E3">
+        <v>399</v>
+      </c>
+      <c r="F3">
+        <v>444</v>
+      </c>
+      <c r="G3">
+        <v>374</v>
+      </c>
+      <c r="H3">
+        <v>445</v>
+      </c>
+      <c r="I3">
+        <v>509</v>
+      </c>
+      <c r="J3">
+        <v>528</v>
+      </c>
+      <c r="K3">
+        <v>537</v>
+      </c>
+      <c r="L3">
+        <v>537</v>
+      </c>
+      <c r="M3">
+        <v>538</v>
+      </c>
+      <c r="N3">
+        <v>509</v>
+      </c>
+      <c r="O3">
+        <v>534</v>
+      </c>
+      <c r="P3">
+        <v>561</v>
+      </c>
+      <c r="Q3">
+        <v>607</v>
+      </c>
+      <c r="R3">
+        <v>189</v>
+      </c>
+      <c r="S3">
+        <v>242</v>
+      </c>
+      <c r="T3">
+        <v>437</v>
+      </c>
+      <c r="U3">
+        <v>648</v>
+      </c>
+      <c r="V3">
+        <v>682</v>
+      </c>
+      <c r="W3" s="23">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4">
+        <v>66.7</v>
+      </c>
+      <c r="C4">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="D4">
+        <v>76.2</v>
+      </c>
+      <c r="E4">
+        <v>84.1</v>
+      </c>
+      <c r="F4">
+        <v>87.9</v>
+      </c>
+      <c r="G4">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="H4">
+        <v>88.6</v>
+      </c>
+      <c r="I4">
+        <v>96.1</v>
+      </c>
+      <c r="J4">
+        <v>95.1</v>
+      </c>
+      <c r="K4">
+        <v>92.1</v>
+      </c>
+      <c r="L4">
+        <v>92.9</v>
+      </c>
+      <c r="M4">
+        <v>83.8</v>
+      </c>
+      <c r="N4">
+        <v>80.8</v>
+      </c>
+      <c r="O4">
+        <v>95.9</v>
+      </c>
+      <c r="P4">
+        <v>111.3</v>
+      </c>
+      <c r="Q4">
+        <v>101</v>
+      </c>
+      <c r="R4">
+        <v>140</v>
+      </c>
+      <c r="S4">
+        <v>210</v>
+      </c>
+      <c r="T4">
+        <v>206</v>
+      </c>
+      <c r="U4">
+        <v>139</v>
+      </c>
+      <c r="V4">
+        <v>149</v>
+      </c>
+      <c r="W4" s="23">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="31">
+        <f>(B3/(B3+B4))*B2</f>
+        <v>308.91599667313557</v>
+      </c>
+      <c r="C5" s="31">
+        <f t="shared" ref="C5:W5" si="0">(C3/(C3+C4))*C2</f>
+        <v>340.6511746680286</v>
+      </c>
+      <c r="D5" s="31">
+        <f t="shared" si="0"/>
+        <v>384.6894832275612</v>
+      </c>
+      <c r="E5" s="31">
+        <f t="shared" si="0"/>
+        <v>421.21713930863172</v>
+      </c>
+      <c r="F5" s="31">
+        <f t="shared" si="0"/>
+        <v>475.80372250423017</v>
+      </c>
+      <c r="G5" s="31">
+        <f t="shared" si="0"/>
+        <v>400.4138551506972</v>
+      </c>
+      <c r="H5" s="31">
+        <f t="shared" si="0"/>
+        <v>470.35232383808096</v>
+      </c>
+      <c r="I5" s="31">
+        <f t="shared" si="0"/>
+        <v>540.03966286564207</v>
+      </c>
+      <c r="J5" s="31">
+        <f t="shared" si="0"/>
+        <v>598.24747231584013</v>
+      </c>
+      <c r="K5" s="31">
+        <f t="shared" si="0"/>
+        <v>614.59227467811161</v>
+      </c>
+      <c r="L5" s="31">
+        <f t="shared" si="0"/>
+        <v>653.8799809493571</v>
+      </c>
+      <c r="M5" s="31">
+        <f t="shared" si="0"/>
+        <v>623.83081376648443</v>
+      </c>
+      <c r="N5" s="31">
+        <f t="shared" si="0"/>
+        <v>611.87012546625976</v>
+      </c>
+      <c r="O5" s="31">
+        <f t="shared" si="0"/>
+        <v>639.20622321003339</v>
+      </c>
+      <c r="P5" s="31">
+        <f t="shared" si="0"/>
+        <v>677.57251227130746</v>
+      </c>
+      <c r="Q5" s="31">
+        <f t="shared" si="0"/>
+        <v>718.45480225988706</v>
+      </c>
+      <c r="R5" s="31">
+        <f t="shared" si="0"/>
+        <v>220.59574468085108</v>
+      </c>
+      <c r="S5" s="31">
+        <f t="shared" si="0"/>
+        <v>274.65929203539827</v>
+      </c>
+      <c r="T5" s="31">
+        <f t="shared" si="0"/>
+        <v>501.56454121306376</v>
+      </c>
+      <c r="U5" s="31">
+        <f t="shared" si="0"/>
+        <v>748.45235069885632</v>
+      </c>
+      <c r="V5" s="31">
+        <f t="shared" si="0"/>
+        <v>792.79422382671476</v>
+      </c>
+      <c r="W5" s="31">
+        <f t="shared" si="0"/>
+        <v>812.51137724550892</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="24">
+        <v>3608.71</v>
+      </c>
+      <c r="C6" s="24">
+        <v>3913.61</v>
+      </c>
+      <c r="D6" s="24">
+        <v>4164.8</v>
+      </c>
+      <c r="E6" s="24">
+        <v>4513.1000000000004</v>
+      </c>
+      <c r="F6" s="24">
+        <v>4608.47</v>
+      </c>
+      <c r="G6" s="24">
+        <v>4561.41</v>
+      </c>
+      <c r="H6" s="24">
+        <v>4930.25</v>
+      </c>
+      <c r="I6" s="24">
+        <v>5254.56</v>
+      </c>
+      <c r="J6" s="24">
+        <v>5535.64</v>
+      </c>
+      <c r="K6" s="24">
+        <v>5839.7</v>
+      </c>
+      <c r="L6" s="24">
+        <v>6188.74</v>
+      </c>
+      <c r="M6" s="24">
+        <v>6652.79</v>
+      </c>
+      <c r="N6" s="24">
+        <v>7144.5</v>
+      </c>
+      <c r="O6" s="24">
+        <v>7716.54</v>
+      </c>
+      <c r="P6" s="24">
+        <v>8278.7800000000007</v>
+      </c>
+      <c r="Q6">
+        <v>8688</v>
+      </c>
+      <c r="R6">
+        <v>2974</v>
+      </c>
+      <c r="S6">
+        <v>3623</v>
+      </c>
+      <c r="T6">
+        <v>5974</v>
+      </c>
+      <c r="U6">
+        <v>8271</v>
+      </c>
+      <c r="V6">
+        <v>9082</v>
+      </c>
+      <c r="W6" s="23">
+        <f>V6*(1.058)</f>
+        <v>9608.7560000000012</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7">
+        <v>73.7</v>
+      </c>
+      <c r="C7">
+        <v>75.2</v>
+      </c>
+      <c r="D7">
+        <v>76.3</v>
+      </c>
+      <c r="E7">
+        <v>77.3</v>
+      </c>
+      <c r="F7">
+        <v>76.3</v>
+      </c>
+      <c r="G7">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="H7">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="I7">
+        <v>78.7</v>
+      </c>
+      <c r="J7">
+        <v>79.5</v>
+      </c>
+      <c r="K7">
+        <v>79.900000000000006</v>
+      </c>
+      <c r="L7">
+        <v>80</v>
+      </c>
+      <c r="M7">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="N7">
+        <v>80.5</v>
+      </c>
+      <c r="O7">
+        <v>81.5</v>
+      </c>
+      <c r="P7">
+        <v>81.7</v>
+      </c>
+      <c r="Q7">
+        <v>82.6</v>
+      </c>
+      <c r="R7">
+        <v>65.2</v>
+      </c>
+      <c r="S7">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="T7">
+        <v>78.7</v>
+      </c>
+      <c r="U7">
+        <v>82.2</v>
+      </c>
+      <c r="V7">
+        <v>83.5</v>
+      </c>
+      <c r="W7" s="23">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="31">
+        <f>B6/B7*100</f>
+        <v>4896.4857530529171</v>
+      </c>
+      <c r="C8" s="31">
+        <f t="shared" ref="C8:W8" si="1">C6/C7*100</f>
+        <v>5204.2686170212764</v>
+      </c>
+      <c r="D8" s="31">
+        <f t="shared" si="1"/>
+        <v>5458.4534731323729</v>
+      </c>
+      <c r="E8" s="31">
+        <f t="shared" si="1"/>
+        <v>5838.421733505822</v>
+      </c>
+      <c r="F8" s="31">
+        <f t="shared" si="1"/>
+        <v>6039.9344692005252</v>
+      </c>
+      <c r="G8" s="31">
+        <f t="shared" si="1"/>
+        <v>5970.4319371727743</v>
+      </c>
+      <c r="H8" s="31">
+        <f t="shared" si="1"/>
+        <v>6248.7325728770593</v>
+      </c>
+      <c r="I8" s="31">
+        <f t="shared" si="1"/>
+        <v>6676.6963151207119</v>
+      </c>
+      <c r="J8" s="31">
+        <f t="shared" si="1"/>
+        <v>6963.0691823899369</v>
+      </c>
+      <c r="K8" s="31">
+        <f t="shared" si="1"/>
+        <v>7308.760951188985</v>
+      </c>
+      <c r="L8" s="31">
+        <f t="shared" si="1"/>
+        <v>7735.9250000000002</v>
+      </c>
+      <c r="M8" s="31">
+        <f t="shared" si="1"/>
+        <v>8254.0818858560797</v>
+      </c>
+      <c r="N8" s="31">
+        <f t="shared" si="1"/>
+        <v>8875.1552795031057</v>
+      </c>
+      <c r="O8" s="31">
+        <f t="shared" si="1"/>
+        <v>9468.1472392638043</v>
+      </c>
+      <c r="P8" s="31">
+        <f t="shared" si="1"/>
+        <v>10133.145654834761</v>
+      </c>
+      <c r="Q8" s="31">
+        <f t="shared" si="1"/>
+        <v>10518.159806295402</v>
+      </c>
+      <c r="R8" s="31">
+        <f t="shared" si="1"/>
+        <v>4561.3496932515336</v>
+      </c>
+      <c r="S8" s="31">
+        <f t="shared" si="1"/>
+        <v>5415.5455904334822</v>
+      </c>
+      <c r="T8" s="31">
+        <f t="shared" si="1"/>
+        <v>7590.8513341804319</v>
+      </c>
+      <c r="U8" s="31">
+        <f t="shared" si="1"/>
+        <v>10062.043795620437</v>
+      </c>
+      <c r="V8" s="31">
+        <f t="shared" si="1"/>
+        <v>10876.646706586827</v>
+      </c>
+      <c r="W8" s="31">
+        <f t="shared" si="1"/>
+        <v>11438.99523809524</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="31">
+        <f>B3/B6</f>
+        <v>8.1469555602971699E-2</v>
+      </c>
+      <c r="C9" s="31">
+        <f t="shared" ref="C9:W9" si="2">C3/C6</f>
+        <v>8.2532495573140907E-2</v>
+      </c>
+      <c r="D9" s="31">
+        <f t="shared" si="2"/>
+        <v>8.7639262389550512E-2</v>
+      </c>
+      <c r="E9" s="31">
+        <f t="shared" si="2"/>
+        <v>8.8409297378741883E-2</v>
+      </c>
+      <c r="F9" s="31">
+        <f t="shared" si="2"/>
+        <v>9.6344339878528015E-2</v>
+      </c>
+      <c r="G9" s="31">
+        <f t="shared" si="2"/>
+        <v>8.1992191011112797E-2</v>
+      </c>
+      <c r="H9" s="31">
+        <f t="shared" si="2"/>
+        <v>9.0259114649358554E-2</v>
+      </c>
+      <c r="I9" s="31">
+        <f t="shared" si="2"/>
+        <v>9.6868243963338499E-2</v>
+      </c>
+      <c r="J9" s="31">
+        <f t="shared" si="2"/>
+        <v>9.5381925125188768E-2</v>
+      </c>
+      <c r="K9" s="31">
+        <f t="shared" si="2"/>
+        <v>9.1956778601640504E-2</v>
+      </c>
+      <c r="L9" s="31">
+        <f t="shared" si="2"/>
+        <v>8.6770489631168873E-2</v>
+      </c>
+      <c r="M9" s="31">
+        <f t="shared" si="2"/>
+        <v>8.0868327423532088E-2</v>
+      </c>
+      <c r="N9" s="31">
+        <f t="shared" si="2"/>
+        <v>7.1243613968787173E-2</v>
+      </c>
+      <c r="O9" s="31">
+        <f t="shared" si="2"/>
+        <v>6.92019998600409E-2</v>
+      </c>
+      <c r="P9" s="31">
+        <f t="shared" si="2"/>
+        <v>6.7763607681325028E-2</v>
+      </c>
+      <c r="Q9" s="31">
+        <f t="shared" si="2"/>
+        <v>6.9866482504604047E-2</v>
+      </c>
+      <c r="R9" s="31">
+        <f t="shared" si="2"/>
+        <v>6.3550773369199731E-2</v>
+      </c>
+      <c r="S9" s="31">
+        <f t="shared" si="2"/>
+        <v>6.6795473364614957E-2</v>
+      </c>
+      <c r="T9" s="31">
+        <f t="shared" si="2"/>
+        <v>7.3150318044861065E-2</v>
+      </c>
+      <c r="U9" s="31">
+        <f t="shared" si="2"/>
+        <v>7.8346028291621322E-2</v>
+      </c>
+      <c r="V9" s="31">
+        <f t="shared" si="2"/>
+        <v>7.5093591719885486E-2</v>
+      </c>
+      <c r="W9" s="31">
+        <f t="shared" si="2"/>
+        <v>7.2121718982145019E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="31">
+        <f>B5/B6</f>
+        <v>8.5602887644930056E-2</v>
+      </c>
+      <c r="C10" s="31">
+        <f t="shared" ref="C10:W10" si="3">C5/C6</f>
+        <v>8.7042698344502539E-2</v>
+      </c>
+      <c r="D10" s="31">
+        <f t="shared" si="3"/>
+        <v>9.2366856326248845E-2</v>
+      </c>
+      <c r="E10" s="31">
+        <f t="shared" si="3"/>
+        <v>9.3332108596891644E-2</v>
+      </c>
+      <c r="F10" s="31">
+        <f t="shared" si="3"/>
+        <v>0.10324548548742428</v>
+      </c>
+      <c r="G10" s="31">
+        <f t="shared" si="3"/>
+        <v>8.7782912553508063E-2</v>
+      </c>
+      <c r="H10" s="31">
+        <f t="shared" si="3"/>
+        <v>9.5401313085154094E-2</v>
+      </c>
+      <c r="I10" s="31">
+        <f t="shared" si="3"/>
+        <v>0.10277542988673495</v>
+      </c>
+      <c r="J10" s="31">
+        <f t="shared" si="3"/>
+        <v>0.10807196138402066</v>
+      </c>
+      <c r="K10" s="31">
+        <f t="shared" si="3"/>
+        <v>0.10524380955838684</v>
+      </c>
+      <c r="L10" s="31">
+        <f t="shared" si="3"/>
+        <v>0.10565639870948806</v>
+      </c>
+      <c r="M10" s="31">
+        <f t="shared" si="3"/>
+        <v>9.3769803911815108E-2</v>
+      </c>
+      <c r="N10" s="31">
+        <f t="shared" si="3"/>
+        <v>8.5642119877704495E-2</v>
+      </c>
+      <c r="O10" s="31">
+        <f t="shared" si="3"/>
+        <v>8.283585949273034E-2</v>
+      </c>
+      <c r="P10" s="31">
+        <f t="shared" si="3"/>
+        <v>8.184448823030778E-2</v>
+      </c>
+      <c r="Q10" s="31">
+        <f t="shared" si="3"/>
+        <v>8.2695073924940965E-2</v>
+      </c>
+      <c r="R10" s="31">
+        <f t="shared" si="3"/>
+        <v>7.4174762838214892E-2</v>
+      </c>
+      <c r="S10" s="31">
+        <f t="shared" si="3"/>
+        <v>7.5809906716919201E-2</v>
+      </c>
+      <c r="T10" s="31">
+        <f t="shared" si="3"/>
+        <v>8.3957907802655468E-2</v>
+      </c>
+      <c r="U10" s="31">
+        <f t="shared" si="3"/>
+        <v>9.0491155930220807E-2</v>
+      </c>
+      <c r="V10" s="31">
+        <f t="shared" si="3"/>
+        <v>8.7292911674379511E-2</v>
+      </c>
+      <c r="W10" s="31">
+        <f t="shared" si="3"/>
+        <v>8.4559476507209547E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11">
+        <v>1994</v>
+      </c>
+      <c r="C11">
+        <v>2135</v>
+      </c>
+      <c r="D11">
+        <v>2255</v>
+      </c>
+      <c r="E11">
+        <v>2452</v>
+      </c>
+      <c r="F11">
+        <v>2489</v>
+      </c>
+      <c r="G11">
+        <v>2479</v>
+      </c>
+      <c r="H11">
+        <v>2695</v>
+      </c>
+      <c r="I11">
+        <v>2859</v>
+      </c>
+      <c r="J11">
+        <v>2991</v>
+      </c>
+      <c r="K11">
+        <v>3143</v>
+      </c>
+      <c r="L11">
+        <v>3326</v>
+      </c>
+      <c r="M11">
+        <v>3565</v>
+      </c>
+      <c r="N11">
+        <v>3815</v>
+      </c>
+      <c r="O11">
+        <v>4093</v>
+      </c>
+      <c r="P11">
+        <v>4378</v>
+      </c>
+      <c r="Q11">
+        <v>4560</v>
+      </c>
+      <c r="R11">
+        <v>1779</v>
+      </c>
+      <c r="S11">
+        <v>2304</v>
+      </c>
+      <c r="T11">
+        <v>3452</v>
+      </c>
+      <c r="U11">
+        <v>4426</v>
+      </c>
+      <c r="V11">
+        <v>4779</v>
+      </c>
+      <c r="W11" s="23">
+        <v>4988</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12">
+        <v>40.9</v>
+      </c>
+      <c r="C12">
+        <v>41.9</v>
+      </c>
+      <c r="D12">
+        <v>44.6</v>
+      </c>
+      <c r="E12">
+        <v>46.7</v>
+      </c>
+      <c r="F12">
+        <v>46.4</v>
+      </c>
+      <c r="G12">
+        <v>42.3</v>
+      </c>
+      <c r="H12">
+        <v>50.5</v>
+      </c>
+      <c r="I12">
+        <v>50.7</v>
+      </c>
+      <c r="J12">
+        <v>50.7</v>
+      </c>
+      <c r="K12">
+        <v>51.7</v>
+      </c>
+      <c r="L12">
+        <v>54</v>
+      </c>
+      <c r="M12">
+        <v>54.8</v>
+      </c>
+      <c r="N12">
+        <v>57</v>
+      </c>
+      <c r="O12">
+        <v>61.5</v>
+      </c>
+      <c r="P12">
+        <v>63.3</v>
+      </c>
+      <c r="W12" s="23"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>3.5</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>1.5</v>
+      </c>
+      <c r="G13">
+        <v>-2</v>
+      </c>
+      <c r="H13">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I13">
+        <v>2.5</v>
+      </c>
+      <c r="J13">
+        <v>2.5</v>
+      </c>
+      <c r="K13">
+        <v>2.7</v>
+      </c>
+      <c r="L13">
+        <v>2.7</v>
+      </c>
+      <c r="M13">
+        <v>3.2</v>
+      </c>
+      <c r="N13">
+        <v>3.4</v>
+      </c>
+      <c r="O13">
+        <v>3.4</v>
+      </c>
+      <c r="P13">
+        <v>3.1</v>
+      </c>
+      <c r="Q13">
+        <v>2.9</v>
+      </c>
+      <c r="R13">
+        <v>-2.7</v>
+      </c>
+      <c r="S13">
+        <v>6.6</v>
+      </c>
+      <c r="T13">
+        <v>3.6</v>
+      </c>
+      <c r="U13">
+        <v>3.5</v>
+      </c>
+      <c r="V13">
+        <v>3.3</v>
+      </c>
+      <c r="W13" s="23">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14">
+        <v>376</v>
+      </c>
+      <c r="C14">
+        <v>409</v>
+      </c>
+      <c r="D14">
+        <v>450</v>
+      </c>
+      <c r="E14">
+        <v>490</v>
+      </c>
+      <c r="F14">
+        <v>571</v>
+      </c>
+      <c r="G14">
+        <v>474</v>
+      </c>
+      <c r="H14">
+        <v>536</v>
+      </c>
+      <c r="I14">
+        <v>623</v>
+      </c>
+      <c r="J14">
+        <v>687</v>
+      </c>
+      <c r="K14">
+        <v>695</v>
+      </c>
+      <c r="L14">
+        <v>731</v>
+      </c>
+      <c r="M14">
+        <v>659</v>
+      </c>
+      <c r="N14">
+        <v>649</v>
+      </c>
+      <c r="O14">
+        <v>697</v>
+      </c>
+      <c r="P14">
+        <v>766</v>
+      </c>
+      <c r="Q14">
+        <v>795</v>
+      </c>
+      <c r="R14">
+        <v>495</v>
+      </c>
+      <c r="S14">
+        <v>556</v>
+      </c>
+      <c r="T14">
+        <v>727</v>
+      </c>
+      <c r="U14">
+        <v>846</v>
+      </c>
+      <c r="V14">
+        <v>904</v>
+      </c>
+      <c r="W14" s="23">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="31">
+        <f>(B3/(B3+B4))*B14</f>
+        <v>306.47075131688388</v>
+      </c>
+      <c r="C15" s="31">
+        <f t="shared" ref="C15:W15" si="4">(C3/(C3+C4))*C14</f>
+        <v>337.35188968335035</v>
+      </c>
+      <c r="D15" s="31">
+        <f t="shared" si="4"/>
+        <v>372.2801450589302</v>
+      </c>
+      <c r="E15" s="31">
+        <f t="shared" si="4"/>
+        <v>404.69882012005792</v>
+      </c>
+      <c r="F15" s="31">
+        <f t="shared" si="4"/>
+        <v>476.63846587704461</v>
+      </c>
+      <c r="G15" s="31">
+        <f t="shared" si="4"/>
+        <v>398.73144399460188</v>
+      </c>
+      <c r="H15" s="31">
+        <f t="shared" si="4"/>
+        <v>447.00149925037482</v>
+      </c>
+      <c r="I15" s="31">
+        <f t="shared" si="4"/>
+        <v>524.05718063130064</v>
+      </c>
+      <c r="J15" s="31">
+        <f t="shared" si="4"/>
+        <v>582.14732787674529</v>
+      </c>
+      <c r="K15" s="31">
+        <f t="shared" si="4"/>
+        <v>593.25226514067708</v>
+      </c>
+      <c r="L15" s="31">
+        <f t="shared" si="4"/>
+        <v>623.18939514208603</v>
+      </c>
+      <c r="M15" s="31">
+        <f t="shared" si="4"/>
+        <v>570.18655516243166</v>
+      </c>
+      <c r="N15" s="31">
+        <f t="shared" si="4"/>
+        <v>560.08986096982039</v>
+      </c>
+      <c r="O15" s="31">
+        <f t="shared" si="4"/>
+        <v>590.88426734402287</v>
+      </c>
+      <c r="P15" s="31">
+        <f t="shared" si="4"/>
+        <v>639.1878625613565</v>
+      </c>
+      <c r="Q15" s="31">
+        <f t="shared" si="4"/>
+        <v>681.58898305084745</v>
+      </c>
+      <c r="R15" s="31">
+        <f t="shared" si="4"/>
+        <v>284.36170212765961</v>
+      </c>
+      <c r="S15" s="31">
+        <f t="shared" si="4"/>
+        <v>297.68141592920358</v>
+      </c>
+      <c r="T15" s="31">
+        <f t="shared" si="4"/>
+        <v>494.08864696734059</v>
+      </c>
+      <c r="U15" s="31">
+        <f t="shared" si="4"/>
+        <v>696.57941550190594</v>
+      </c>
+      <c r="V15" s="31">
+        <f t="shared" si="4"/>
+        <v>741.91095066185312</v>
+      </c>
+      <c r="W15" s="31">
+        <f t="shared" si="4"/>
+        <v>757.73532934131731</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="31">
+        <f>B15/B6</f>
+        <v>8.4925292228215585E-2</v>
+      </c>
+      <c r="C16" s="31">
+        <f t="shared" ref="C16:W16" si="5">C15/C6</f>
+        <v>8.6199669789107841E-2</v>
+      </c>
+      <c r="D16" s="31">
+        <f t="shared" si="5"/>
+        <v>8.9387280315724696E-2</v>
+      </c>
+      <c r="E16" s="31">
+        <f t="shared" si="5"/>
+        <v>8.9672025906817457E-2</v>
+      </c>
+      <c r="F16" s="31">
+        <f t="shared" si="5"/>
+        <v>0.10342661791810397</v>
+      </c>
+      <c r="G16" s="31">
+        <f t="shared" si="5"/>
+        <v>8.741407678647653E-2</v>
+      </c>
+      <c r="H16" s="31">
+        <f t="shared" si="5"/>
+        <v>9.0665077683763459E-2</v>
+      </c>
+      <c r="I16" s="31">
+        <f t="shared" si="5"/>
+        <v>9.9733789438373646E-2</v>
+      </c>
+      <c r="J16" s="31">
+        <f t="shared" si="5"/>
+        <v>0.10516350916547053</v>
+      </c>
+      <c r="K16" s="31">
+        <f t="shared" si="5"/>
+        <v>0.10158951061538728</v>
+      </c>
+      <c r="L16" s="31">
+        <f t="shared" si="5"/>
+        <v>0.10069729785741299</v>
+      </c>
+      <c r="M16" s="31">
+        <f t="shared" si="5"/>
+        <v>8.570638110663821E-2</v>
+      </c>
+      <c r="N16" s="31">
+        <f t="shared" si="5"/>
+        <v>7.8394549789323309E-2</v>
+      </c>
+      <c r="O16" s="31">
+        <f t="shared" si="5"/>
+        <v>7.6573732183598198E-2</v>
+      </c>
+      <c r="P16" s="31">
+        <f t="shared" si="5"/>
+        <v>7.7207977813319895E-2</v>
+      </c>
+      <c r="Q16" s="31">
+        <f t="shared" si="5"/>
+        <v>7.8451770608983368E-2</v>
+      </c>
+      <c r="R16" s="31">
+        <f t="shared" si="5"/>
+        <v>9.5615905221136388E-2</v>
+      </c>
+      <c r="S16" s="31">
+        <f t="shared" si="5"/>
+        <v>8.2164343342313984E-2</v>
+      </c>
+      <c r="T16" s="31">
+        <f t="shared" si="5"/>
+        <v>8.270650267280559E-2</v>
+      </c>
+      <c r="U16" s="31">
+        <f t="shared" si="5"/>
+        <v>8.4219491657829271E-2</v>
+      </c>
+      <c r="V16" s="31">
+        <f t="shared" si="5"/>
+        <v>8.1690261028611877E-2</v>
+      </c>
+      <c r="W16" s="31">
+        <f t="shared" si="5"/>
+        <v>7.8858837641554977E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A17" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17">
+        <v>65</v>
+      </c>
+      <c r="C17">
+        <v>91</v>
+      </c>
+      <c r="D17">
+        <v>127</v>
+      </c>
+      <c r="E17">
+        <v>146</v>
+      </c>
+      <c r="F17">
+        <v>203</v>
+      </c>
+      <c r="G17">
+        <v>134</v>
+      </c>
+      <c r="H17">
+        <v>151</v>
+      </c>
+      <c r="I17">
+        <v>191</v>
+      </c>
+      <c r="J17">
+        <v>228</v>
+      </c>
+      <c r="K17">
+        <v>230</v>
+      </c>
+      <c r="L17">
+        <v>224</v>
+      </c>
+      <c r="M17">
+        <v>174</v>
+      </c>
+      <c r="N17">
+        <v>135</v>
+      </c>
+      <c r="O17">
+        <v>149</v>
+      </c>
+      <c r="P17">
+        <v>180</v>
+      </c>
+      <c r="Q17">
+        <v>190</v>
+      </c>
+      <c r="R17">
+        <v>80</v>
+      </c>
+      <c r="S17">
+        <v>106</v>
+      </c>
+      <c r="T17">
+        <v>215</v>
+      </c>
+      <c r="U17">
+        <v>269</v>
+      </c>
+      <c r="V17">
+        <v>261</v>
+      </c>
+      <c r="W17" s="23">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A18" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18">
+        <v>49.7</v>
+      </c>
+      <c r="C18">
+        <v>71</v>
+      </c>
+      <c r="D18">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="E18">
+        <v>90</v>
+      </c>
+      <c r="F18">
+        <v>126.7</v>
+      </c>
+      <c r="G18">
+        <v>91.4</v>
+      </c>
+      <c r="H18">
+        <v>112.7</v>
+      </c>
+      <c r="I18">
+        <v>129.6</v>
+      </c>
+      <c r="J18">
+        <v>124.5</v>
+      </c>
+      <c r="K18">
+        <v>114.8</v>
+      </c>
+      <c r="L18">
+        <v>99.9</v>
+      </c>
+      <c r="M18">
+        <v>66.7</v>
+      </c>
+      <c r="N18">
+        <v>52.1</v>
+      </c>
+      <c r="O18">
+        <v>66.7</v>
+      </c>
+      <c r="P18">
+        <v>86.1</v>
+      </c>
+      <c r="Q18">
+        <v>80</v>
+      </c>
+      <c r="R18">
+        <v>47</v>
+      </c>
+      <c r="S18">
+        <v>78</v>
+      </c>
+      <c r="T18">
+        <v>139</v>
+      </c>
+      <c r="U18">
+        <v>112</v>
+      </c>
+      <c r="V18">
+        <v>99</v>
+      </c>
+      <c r="W18" s="23">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A19" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19">
+        <v>311</v>
+      </c>
+      <c r="C19">
+        <v>318</v>
+      </c>
+      <c r="D19">
+        <v>324</v>
+      </c>
+      <c r="E19">
+        <v>344</v>
+      </c>
+      <c r="F19">
+        <v>367</v>
+      </c>
+      <c r="G19">
+        <v>340</v>
+      </c>
+      <c r="H19">
+        <v>385</v>
+      </c>
+      <c r="I19">
+        <v>431</v>
+      </c>
+      <c r="J19">
+        <v>459</v>
+      </c>
+      <c r="K19">
+        <v>464</v>
+      </c>
+      <c r="L19">
+        <v>507</v>
+      </c>
+      <c r="M19">
+        <v>485</v>
+      </c>
+      <c r="N19">
+        <v>514</v>
+      </c>
+      <c r="O19">
+        <v>548</v>
+      </c>
+      <c r="P19">
+        <v>586</v>
+      </c>
+      <c r="Q19">
+        <v>605</v>
+      </c>
+      <c r="R19">
+        <v>415</v>
+      </c>
+      <c r="S19">
+        <v>450</v>
+      </c>
+      <c r="T19">
+        <v>512</v>
+      </c>
+      <c r="U19">
+        <v>577</v>
+      </c>
+      <c r="V19">
+        <v>643</v>
+      </c>
+      <c r="W19" s="23">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A20" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20">
+        <v>3.3</v>
+      </c>
+      <c r="C20">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D20">
+        <v>15</v>
+      </c>
+      <c r="E20">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="F20">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="G20">
+        <v>1.9</v>
+      </c>
+      <c r="H20">
+        <v>27.6</v>
+      </c>
+      <c r="I20">
+        <v>19.8</v>
+      </c>
+      <c r="J20">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="K20">
+        <v>25.3</v>
+      </c>
+      <c r="L20">
+        <v>35.5</v>
+      </c>
+      <c r="M20">
+        <v>62</v>
+      </c>
+      <c r="N20">
+        <v>60.1</v>
+      </c>
+      <c r="O20">
+        <v>56.3</v>
+      </c>
+      <c r="P20">
+        <v>45.9</v>
+      </c>
+      <c r="Q20">
+        <v>43.1</v>
+      </c>
+      <c r="R20">
+        <v>-110.9</v>
+      </c>
+      <c r="S20">
+        <v>-43.5</v>
+      </c>
+      <c r="T20">
+        <v>11.3</v>
+      </c>
+      <c r="U20">
+        <v>62.9</v>
+      </c>
+      <c r="V20">
+        <v>61.9</v>
+      </c>
+      <c r="W20" s="23">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A21" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21">
+        <v>0.9</v>
+      </c>
+      <c r="C21">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D21">
+        <v>3.2</v>
+      </c>
+      <c r="E21">
+        <v>3.9</v>
+      </c>
+      <c r="F21">
+        <v>-0.2</v>
+      </c>
+      <c r="G21">
+        <v>0.4</v>
+      </c>
+      <c r="H21">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I21">
+        <v>3.1</v>
+      </c>
+      <c r="J21">
+        <v>2.6</v>
+      </c>
+      <c r="K21">
+        <v>3.5</v>
+      </c>
+      <c r="L21">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="M21">
+        <v>8.6</v>
+      </c>
+      <c r="N21">
+        <v>8.5</v>
+      </c>
+      <c r="O21">
+        <v>7.5</v>
+      </c>
+      <c r="P21">
+        <v>5.7</v>
+      </c>
+      <c r="Q21">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="R21">
+        <v>-28.8</v>
+      </c>
+      <c r="S21">
+        <v>-8.5</v>
+      </c>
+      <c r="T21">
+        <v>1.5</v>
+      </c>
+      <c r="U21">
+        <v>6.9</v>
+      </c>
+      <c r="V21">
+        <v>6.4</v>
+      </c>
+      <c r="W21" s="23">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A22" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22">
+        <v>-5.6</v>
+      </c>
+      <c r="C22">
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>14.7</v>
+      </c>
+      <c r="F22">
+        <v>-26.1</v>
+      </c>
+      <c r="G22">
+        <v>-4.5999999999999996</v>
+      </c>
+      <c r="H22">
+        <v>17.3</v>
+      </c>
+      <c r="I22">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J22">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="K22">
+        <v>10.7</v>
+      </c>
+      <c r="L22">
+        <v>13.8</v>
+      </c>
+      <c r="M22">
+        <v>36</v>
+      </c>
+      <c r="N22">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="O22">
+        <v>38</v>
+      </c>
+      <c r="P22">
+        <v>27.3</v>
+      </c>
+      <c r="Q22">
+        <v>26.4</v>
+      </c>
+      <c r="R22">
+        <v>-138.69999999999999</v>
+      </c>
+      <c r="S22">
+        <v>-40.4</v>
+      </c>
+      <c r="T22">
+        <v>-3.5</v>
+      </c>
+      <c r="U22">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="V22">
+        <v>32.4</v>
+      </c>
+      <c r="W22" s="23">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A23" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="25">
+        <v>-1.5</v>
+      </c>
+      <c r="C23" s="25">
+        <v>-1</v>
+      </c>
+      <c r="D23" s="25">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E23" s="25">
+        <v>2.9</v>
+      </c>
+      <c r="F23" s="25">
+        <v>-4.5999999999999996</v>
+      </c>
+      <c r="G23" s="25">
+        <v>-1</v>
+      </c>
+      <c r="H23" s="25">
+        <v>3.1</v>
+      </c>
+      <c r="I23" s="25">
+        <v>1.3</v>
+      </c>
+      <c r="J23" s="25">
+        <v>1.3</v>
+      </c>
+      <c r="K23" s="25">
+        <v>1.5</v>
+      </c>
+      <c r="L23" s="25">
+        <v>1.8</v>
+      </c>
+      <c r="M23" s="25">
+        <v>5</v>
+      </c>
+      <c r="N23" s="25">
+        <v>4.8</v>
+      </c>
+      <c r="O23" s="25">
+        <v>5</v>
+      </c>
+      <c r="P23" s="25">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="Q23" s="25">
+        <v>3.1</v>
+      </c>
+      <c r="R23" s="25">
+        <v>-35.799999999999997</v>
+      </c>
+      <c r="S23" s="25">
+        <v>-7.9</v>
+      </c>
+      <c r="T23" s="25">
+        <v>-0.5</v>
+      </c>
+      <c r="U23" s="25">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="V23" s="25">
+        <v>3.4</v>
+      </c>
+      <c r="W23" s="26">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="V24" t="s">
+        <v>70</v>
+      </c>
+      <c r="W24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>66</v>
+      </c>
+      <c r="C60" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finished work on written project
</commit_message>
<xml_diff>
--- a/aeromaps/resources/cost_data/IATA_cost_data.xlsx
+++ b/aeromaps/resources/cost_data/IATA_cost_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a.salgas/PycharmProjects/AeroMAPS/aeromaps/resources/cost_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7C77A3-7011-6943-B8F1-B7D3C0D0B920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16913DF4-3D19-9249-8098-E3AE0DA7B18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29560" yWindow="-8760" windowWidth="38080" windowHeight="20780" activeTab="1" xr2:uid="{21AF616A-B21B-4352-988D-7E50970EE7EE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="83">
   <si>
     <t>Station expenses</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>Avg cost, $/RPK</t>
+  </si>
+  <si>
+    <t>Cargo + anx (share), $ billion</t>
+  </si>
+  <si>
+    <t>Cargo + anx (share) expenses, $ billion</t>
   </si>
 </sst>
 </file>
@@ -687,6 +693,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -696,8 +704,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -907,7 +913,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Exploration!$B$23:$W$23</c:f>
+              <c:f>Exploration!$B$25:$W$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
@@ -1094,7 +1100,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Exploration!$B$21:$W$21</c:f>
+              <c:f>Exploration!$B$23:$W$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
@@ -1974,13 +1980,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2054864</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>78740</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>693419</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>78740</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2562,13 +2568,13 @@
     </row>
     <row r="18" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="32"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="34"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="15" t="s">
@@ -2806,11 +2812,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0427CF9A-7727-6944-B3E2-D626E1863BCC}">
-  <dimension ref="A1:W61"/>
+  <dimension ref="A1:W63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A30" sqref="A30"/>
+      <selection pane="topRight" activeCell="I15" sqref="I1:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2818,7 +2824,7 @@
     <col min="1" max="1" width="31.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="27"/>
       <c r="B1" s="21">
         <v>2004</v>
@@ -2887,7 +2893,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
         <v>49</v>
       </c>
@@ -2958,7 +2964,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
         <v>50</v>
       </c>
@@ -3100,1508 +3106,1694 @@
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+    <row r="5" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5">
+        <f>B2*(B4/(B4+B3))</f>
+        <v>70.084003326864433</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:W5" si="0">C2*(C4/(C4+C3))</f>
+        <v>72.348825331971398</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>80.310516772438802</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>88.782860691368242</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>94.196277495769891</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>75.586144849302727</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>93.647676161919023</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>101.96033713435796</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>107.75252768415983</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>105.40772532188841</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>113.12001905064297</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>97.169186233515603</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>97.129874533740249</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>114.79377678996667</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>134.42748772869257</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>119.54519774011298</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="0"/>
+        <v>163.40425531914894</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="0"/>
+        <v>238.34070796460176</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="0"/>
+        <v>236.43545878693624</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="0"/>
+        <v>160.54764930114357</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="0"/>
+        <v>173.20577617328522</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="0"/>
+        <v>166.48862275449102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" s="31" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="34">
+      <c r="B6" s="31">
         <f>(B3/(B3+B4))*B2</f>
         <v>308.91599667313557</v>
       </c>
-      <c r="C5" s="34">
-        <f t="shared" ref="C5:W5" si="0">(C3/(C3+C4))*C2</f>
+      <c r="C6" s="31">
+        <f t="shared" ref="C6:W6" si="1">(C3/(C3+C4))*C2</f>
         <v>340.6511746680286</v>
       </c>
-      <c r="D5" s="34">
-        <f t="shared" si="0"/>
+      <c r="D6" s="31">
+        <f t="shared" si="1"/>
         <v>384.6894832275612</v>
       </c>
-      <c r="E5" s="34">
-        <f t="shared" si="0"/>
+      <c r="E6" s="31">
+        <f t="shared" si="1"/>
         <v>421.21713930863172</v>
       </c>
-      <c r="F5" s="34">
-        <f t="shared" si="0"/>
+      <c r="F6" s="31">
+        <f t="shared" si="1"/>
         <v>475.80372250423017</v>
       </c>
-      <c r="G5" s="34">
-        <f t="shared" si="0"/>
+      <c r="G6" s="31">
+        <f t="shared" si="1"/>
         <v>400.4138551506972</v>
       </c>
-      <c r="H5" s="34">
-        <f t="shared" si="0"/>
+      <c r="H6" s="31">
+        <f t="shared" si="1"/>
         <v>470.35232383808096</v>
       </c>
-      <c r="I5" s="34">
-        <f t="shared" si="0"/>
+      <c r="I6" s="31">
+        <f t="shared" si="1"/>
         <v>540.03966286564207</v>
       </c>
-      <c r="J5" s="34">
-        <f t="shared" si="0"/>
+      <c r="J6" s="31">
+        <f t="shared" si="1"/>
         <v>598.24747231584013</v>
       </c>
-      <c r="K5" s="34">
-        <f t="shared" si="0"/>
+      <c r="K6" s="31">
+        <f t="shared" si="1"/>
         <v>614.59227467811161</v>
       </c>
-      <c r="L5" s="34">
-        <f t="shared" si="0"/>
+      <c r="L6" s="31">
+        <f t="shared" si="1"/>
         <v>653.8799809493571</v>
       </c>
-      <c r="M5" s="34">
-        <f t="shared" si="0"/>
+      <c r="M6" s="31">
+        <f t="shared" si="1"/>
         <v>623.83081376648443</v>
       </c>
-      <c r="N5" s="34">
-        <f t="shared" si="0"/>
+      <c r="N6" s="31">
+        <f t="shared" si="1"/>
         <v>611.87012546625976</v>
       </c>
-      <c r="O5" s="34">
-        <f t="shared" si="0"/>
+      <c r="O6" s="31">
+        <f t="shared" si="1"/>
         <v>639.20622321003339</v>
       </c>
-      <c r="P5" s="34">
-        <f t="shared" si="0"/>
+      <c r="P6" s="31">
+        <f t="shared" si="1"/>
         <v>677.57251227130746</v>
       </c>
-      <c r="Q5" s="34">
-        <f t="shared" si="0"/>
+      <c r="Q6" s="31">
+        <f t="shared" si="1"/>
         <v>718.45480225988706</v>
       </c>
-      <c r="R5" s="34">
-        <f t="shared" si="0"/>
+      <c r="R6" s="31">
+        <f t="shared" si="1"/>
         <v>220.59574468085108</v>
       </c>
-      <c r="S5" s="34">
-        <f t="shared" si="0"/>
+      <c r="S6" s="31">
+        <f t="shared" si="1"/>
         <v>274.65929203539827</v>
       </c>
-      <c r="T5" s="34">
-        <f t="shared" si="0"/>
+      <c r="T6" s="31">
+        <f t="shared" si="1"/>
         <v>501.56454121306376</v>
       </c>
-      <c r="U5" s="34">
-        <f t="shared" si="0"/>
+      <c r="U6" s="31">
+        <f t="shared" si="1"/>
         <v>748.45235069885632</v>
       </c>
-      <c r="V5" s="34">
-        <f t="shared" si="0"/>
+      <c r="V6" s="31">
+        <f t="shared" si="1"/>
         <v>792.79422382671476</v>
       </c>
-      <c r="W5" s="34">
-        <f t="shared" si="0"/>
+      <c r="W6" s="31">
+        <f t="shared" si="1"/>
         <v>812.51137724550892</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A6" s="28" t="s">
+    <row r="7" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B7" s="24">
         <v>3608.71</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C7" s="24">
         <v>3913.61</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D7" s="24">
         <v>4164.8</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E7" s="24">
         <v>4513.1000000000004</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F7" s="24">
         <v>4608.47</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G7" s="24">
         <v>4561.41</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H7" s="24">
         <v>4930.25</v>
       </c>
-      <c r="I6" s="24">
+      <c r="I7" s="24">
         <v>5254.56</v>
       </c>
-      <c r="J6" s="24">
+      <c r="J7" s="24">
         <v>5535.64</v>
       </c>
-      <c r="K6" s="24">
+      <c r="K7" s="24">
         <v>5839.7</v>
       </c>
-      <c r="L6" s="24">
+      <c r="L7" s="24">
         <v>6188.74</v>
       </c>
-      <c r="M6" s="24">
+      <c r="M7" s="24">
         <v>6652.79</v>
       </c>
-      <c r="N6" s="24">
+      <c r="N7" s="24">
         <v>7144.5</v>
       </c>
-      <c r="O6" s="24">
+      <c r="O7" s="24">
         <v>7716.54</v>
       </c>
-      <c r="P6" s="24">
+      <c r="P7" s="24">
         <v>8278.7800000000007</v>
       </c>
-      <c r="Q6">
+      <c r="Q7">
         <v>8688</v>
       </c>
-      <c r="R6">
+      <c r="R7">
         <v>2974</v>
       </c>
-      <c r="S6">
+      <c r="S7">
         <v>3623</v>
       </c>
-      <c r="T6">
+      <c r="T7">
         <v>5974</v>
       </c>
-      <c r="U6">
+      <c r="U7">
         <v>8271</v>
       </c>
-      <c r="V6">
+      <c r="V7">
         <v>9082</v>
       </c>
-      <c r="W6" s="23">
-        <f>V6*(1.058)</f>
+      <c r="W7" s="23">
+        <f>V7*(1.058)</f>
         <v>9608.7560000000012</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>73.7</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>75.2</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>76.3</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>77.3</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>76.3</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <v>76.400000000000006</v>
       </c>
-      <c r="H7">
+      <c r="H8">
         <v>78.900000000000006</v>
       </c>
-      <c r="I7">
+      <c r="I8">
         <v>78.7</v>
       </c>
-      <c r="J7">
+      <c r="J8">
         <v>79.5</v>
       </c>
-      <c r="K7">
+      <c r="K8">
         <v>79.900000000000006</v>
       </c>
-      <c r="L7">
+      <c r="L8">
         <v>80</v>
       </c>
-      <c r="M7">
+      <c r="M8">
         <v>80.599999999999994</v>
       </c>
-      <c r="N7">
+      <c r="N8">
         <v>80.5</v>
       </c>
-      <c r="O7">
+      <c r="O8">
         <v>81.5</v>
       </c>
-      <c r="P7">
+      <c r="P8">
         <v>81.7</v>
       </c>
-      <c r="Q7">
+      <c r="Q8">
         <v>82.6</v>
       </c>
-      <c r="R7">
+      <c r="R8">
         <v>65.2</v>
       </c>
-      <c r="S7">
+      <c r="S8">
         <v>66.900000000000006</v>
       </c>
-      <c r="T7">
+      <c r="T8">
         <v>78.7</v>
       </c>
-      <c r="U7">
+      <c r="U8">
         <v>82.2</v>
       </c>
-      <c r="V7">
+      <c r="V8">
         <v>83.5</v>
       </c>
-      <c r="W7" s="23">
+      <c r="W8" s="23">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="s">
+    <row r="9" spans="1:23" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="34">
-        <f>B6/B7*100</f>
+      <c r="B9" s="31">
+        <f>B7/B8*100</f>
         <v>4896.4857530529171</v>
       </c>
-      <c r="C8" s="34">
-        <f t="shared" ref="C8:W8" si="1">C6/C7*100</f>
+      <c r="C9" s="31">
+        <f t="shared" ref="C9:W9" si="2">C7/C8*100</f>
         <v>5204.2686170212764</v>
       </c>
-      <c r="D8" s="34">
-        <f t="shared" si="1"/>
+      <c r="D9" s="31">
+        <f t="shared" si="2"/>
         <v>5458.4534731323729</v>
       </c>
-      <c r="E8" s="34">
-        <f t="shared" si="1"/>
+      <c r="E9" s="31">
+        <f t="shared" si="2"/>
         <v>5838.421733505822</v>
       </c>
-      <c r="F8" s="34">
-        <f t="shared" si="1"/>
+      <c r="F9" s="31">
+        <f t="shared" si="2"/>
         <v>6039.9344692005252</v>
       </c>
-      <c r="G8" s="34">
-        <f t="shared" si="1"/>
+      <c r="G9" s="31">
+        <f t="shared" si="2"/>
         <v>5970.4319371727743</v>
       </c>
-      <c r="H8" s="34">
-        <f t="shared" si="1"/>
+      <c r="H9" s="31">
+        <f t="shared" si="2"/>
         <v>6248.7325728770593</v>
       </c>
-      <c r="I8" s="34">
-        <f t="shared" si="1"/>
+      <c r="I9" s="31">
+        <f t="shared" si="2"/>
         <v>6676.6963151207119</v>
       </c>
-      <c r="J8" s="34">
-        <f t="shared" si="1"/>
+      <c r="J9" s="31">
+        <f t="shared" si="2"/>
         <v>6963.0691823899369</v>
       </c>
-      <c r="K8" s="34">
-        <f t="shared" si="1"/>
+      <c r="K9" s="31">
+        <f t="shared" si="2"/>
         <v>7308.760951188985</v>
       </c>
-      <c r="L8" s="34">
-        <f t="shared" si="1"/>
+      <c r="L9" s="31">
+        <f t="shared" si="2"/>
         <v>7735.9250000000002</v>
       </c>
-      <c r="M8" s="34">
-        <f t="shared" si="1"/>
+      <c r="M9" s="31">
+        <f t="shared" si="2"/>
         <v>8254.0818858560797</v>
       </c>
-      <c r="N8" s="34">
-        <f t="shared" si="1"/>
+      <c r="N9" s="31">
+        <f t="shared" si="2"/>
         <v>8875.1552795031057</v>
       </c>
-      <c r="O8" s="34">
-        <f t="shared" si="1"/>
+      <c r="O9" s="31">
+        <f t="shared" si="2"/>
         <v>9468.1472392638043</v>
       </c>
-      <c r="P8" s="34">
-        <f t="shared" si="1"/>
+      <c r="P9" s="31">
+        <f t="shared" si="2"/>
         <v>10133.145654834761</v>
       </c>
-      <c r="Q8" s="34">
-        <f t="shared" si="1"/>
+      <c r="Q9" s="31">
+        <f t="shared" si="2"/>
         <v>10518.159806295402</v>
       </c>
-      <c r="R8" s="34">
-        <f t="shared" si="1"/>
+      <c r="R9" s="31">
+        <f t="shared" si="2"/>
         <v>4561.3496932515336</v>
       </c>
-      <c r="S8" s="34">
-        <f t="shared" si="1"/>
+      <c r="S9" s="31">
+        <f t="shared" si="2"/>
         <v>5415.5455904334822</v>
       </c>
-      <c r="T8" s="34">
-        <f t="shared" si="1"/>
+      <c r="T9" s="31">
+        <f t="shared" si="2"/>
         <v>7590.8513341804319</v>
       </c>
-      <c r="U8" s="34">
-        <f t="shared" si="1"/>
+      <c r="U9" s="31">
+        <f t="shared" si="2"/>
         <v>10062.043795620437</v>
       </c>
-      <c r="V8" s="34">
-        <f t="shared" si="1"/>
+      <c r="V9" s="31">
+        <f t="shared" si="2"/>
         <v>10876.646706586827</v>
       </c>
-      <c r="W8" s="34">
-        <f t="shared" si="1"/>
+      <c r="W9" s="31">
+        <f t="shared" si="2"/>
         <v>11438.99523809524</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="33" t="s">
+    <row r="10" spans="1:23" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="34">
-        <f>B3/B6</f>
+      <c r="B10" s="31">
+        <f>B3/B7</f>
         <v>8.1469555602971699E-2</v>
       </c>
-      <c r="C9" s="34">
-        <f t="shared" ref="C9:W9" si="2">C3/C6</f>
+      <c r="C10" s="31">
+        <f t="shared" ref="C10:W10" si="3">C3/C7</f>
         <v>8.2532495573140907E-2</v>
       </c>
-      <c r="D9" s="34">
-        <f t="shared" si="2"/>
+      <c r="D10" s="31">
+        <f t="shared" si="3"/>
         <v>8.7639262389550512E-2</v>
       </c>
-      <c r="E9" s="34">
-        <f t="shared" si="2"/>
+      <c r="E10" s="31">
+        <f t="shared" si="3"/>
         <v>8.8409297378741883E-2</v>
       </c>
-      <c r="F9" s="34">
-        <f t="shared" si="2"/>
+      <c r="F10" s="31">
+        <f t="shared" si="3"/>
         <v>9.6344339878528015E-2</v>
       </c>
-      <c r="G9" s="34">
-        <f t="shared" si="2"/>
+      <c r="G10" s="31">
+        <f t="shared" si="3"/>
         <v>8.1992191011112797E-2</v>
       </c>
-      <c r="H9" s="34">
-        <f t="shared" si="2"/>
+      <c r="H10" s="31">
+        <f t="shared" si="3"/>
         <v>9.0259114649358554E-2</v>
       </c>
-      <c r="I9" s="34">
-        <f t="shared" si="2"/>
+      <c r="I10" s="31">
+        <f t="shared" si="3"/>
         <v>9.6868243963338499E-2</v>
       </c>
-      <c r="J9" s="34">
-        <f t="shared" si="2"/>
+      <c r="J10" s="31">
+        <f t="shared" si="3"/>
         <v>9.5381925125188768E-2</v>
       </c>
-      <c r="K9" s="34">
-        <f t="shared" si="2"/>
+      <c r="K10" s="31">
+        <f t="shared" si="3"/>
         <v>9.1956778601640504E-2</v>
       </c>
-      <c r="L9" s="34">
-        <f t="shared" si="2"/>
+      <c r="L10" s="31">
+        <f t="shared" si="3"/>
         <v>8.6770489631168873E-2</v>
       </c>
-      <c r="M9" s="34">
-        <f t="shared" si="2"/>
+      <c r="M10" s="31">
+        <f t="shared" si="3"/>
         <v>8.0868327423532088E-2</v>
       </c>
-      <c r="N9" s="34">
-        <f t="shared" si="2"/>
+      <c r="N10" s="31">
+        <f t="shared" si="3"/>
         <v>7.1243613968787173E-2</v>
       </c>
-      <c r="O9" s="34">
-        <f t="shared" si="2"/>
+      <c r="O10" s="31">
+        <f t="shared" si="3"/>
         <v>6.92019998600409E-2</v>
       </c>
-      <c r="P9" s="34">
-        <f t="shared" si="2"/>
+      <c r="P10" s="31">
+        <f t="shared" si="3"/>
         <v>6.7763607681325028E-2</v>
       </c>
-      <c r="Q9" s="34">
-        <f t="shared" si="2"/>
+      <c r="Q10" s="31">
+        <f t="shared" si="3"/>
         <v>6.9866482504604047E-2</v>
       </c>
-      <c r="R9" s="34">
-        <f t="shared" si="2"/>
+      <c r="R10" s="31">
+        <f t="shared" si="3"/>
         <v>6.3550773369199731E-2</v>
       </c>
-      <c r="S9" s="34">
-        <f t="shared" si="2"/>
+      <c r="S10" s="31">
+        <f t="shared" si="3"/>
         <v>6.6795473364614957E-2</v>
       </c>
-      <c r="T9" s="34">
-        <f t="shared" si="2"/>
+      <c r="T10" s="31">
+        <f t="shared" si="3"/>
         <v>7.3150318044861065E-2</v>
       </c>
-      <c r="U9" s="34">
-        <f t="shared" si="2"/>
+      <c r="U10" s="31">
+        <f t="shared" si="3"/>
         <v>7.8346028291621322E-2</v>
       </c>
-      <c r="V9" s="34">
-        <f t="shared" si="2"/>
+      <c r="V10" s="31">
+        <f t="shared" si="3"/>
         <v>7.5093591719885486E-2</v>
       </c>
-      <c r="W9" s="34">
-        <f t="shared" si="2"/>
+      <c r="W10" s="31">
+        <f t="shared" si="3"/>
         <v>7.2121718982145019E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="33" t="s">
+    <row r="11" spans="1:23" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="34">
-        <f>B5/B6</f>
+      <c r="B11" s="31">
+        <f>B6/B7</f>
         <v>8.5602887644930056E-2</v>
       </c>
-      <c r="C10" s="34">
-        <f t="shared" ref="C10:W10" si="3">C5/C6</f>
+      <c r="C11" s="31">
+        <f t="shared" ref="C11:W11" si="4">C6/C7</f>
         <v>8.7042698344502539E-2</v>
       </c>
-      <c r="D10" s="34">
-        <f t="shared" si="3"/>
+      <c r="D11" s="31">
+        <f t="shared" si="4"/>
         <v>9.2366856326248845E-2</v>
       </c>
-      <c r="E10" s="34">
-        <f t="shared" si="3"/>
+      <c r="E11" s="31">
+        <f t="shared" si="4"/>
         <v>9.3332108596891644E-2</v>
       </c>
-      <c r="F10" s="34">
-        <f t="shared" si="3"/>
+      <c r="F11" s="31">
+        <f t="shared" si="4"/>
         <v>0.10324548548742428</v>
       </c>
-      <c r="G10" s="34">
-        <f t="shared" si="3"/>
+      <c r="G11" s="31">
+        <f t="shared" si="4"/>
         <v>8.7782912553508063E-2</v>
       </c>
-      <c r="H10" s="34">
-        <f t="shared" si="3"/>
+      <c r="H11" s="31">
+        <f t="shared" si="4"/>
         <v>9.5401313085154094E-2</v>
       </c>
-      <c r="I10" s="34">
-        <f t="shared" si="3"/>
+      <c r="I11" s="31">
+        <f t="shared" si="4"/>
         <v>0.10277542988673495</v>
       </c>
-      <c r="J10" s="34">
-        <f t="shared" si="3"/>
+      <c r="J11" s="31">
+        <f t="shared" si="4"/>
         <v>0.10807196138402066</v>
       </c>
-      <c r="K10" s="34">
-        <f t="shared" si="3"/>
+      <c r="K11" s="31">
+        <f t="shared" si="4"/>
         <v>0.10524380955838684</v>
       </c>
-      <c r="L10" s="34">
-        <f t="shared" si="3"/>
+      <c r="L11" s="31">
+        <f t="shared" si="4"/>
         <v>0.10565639870948806</v>
       </c>
-      <c r="M10" s="34">
-        <f t="shared" si="3"/>
+      <c r="M11" s="31">
+        <f t="shared" si="4"/>
         <v>9.3769803911815108E-2</v>
       </c>
-      <c r="N10" s="34">
-        <f t="shared" si="3"/>
+      <c r="N11" s="31">
+        <f t="shared" si="4"/>
         <v>8.5642119877704495E-2</v>
       </c>
-      <c r="O10" s="34">
-        <f t="shared" si="3"/>
+      <c r="O11" s="31">
+        <f t="shared" si="4"/>
         <v>8.283585949273034E-2</v>
       </c>
-      <c r="P10" s="34">
-        <f t="shared" si="3"/>
+      <c r="P11" s="31">
+        <f t="shared" si="4"/>
         <v>8.184448823030778E-2</v>
       </c>
-      <c r="Q10" s="34">
-        <f t="shared" si="3"/>
+      <c r="Q11" s="31">
+        <f t="shared" si="4"/>
         <v>8.2695073924940965E-2</v>
       </c>
-      <c r="R10" s="34">
-        <f t="shared" si="3"/>
+      <c r="R11" s="31">
+        <f t="shared" si="4"/>
         <v>7.4174762838214892E-2</v>
       </c>
-      <c r="S10" s="34">
-        <f t="shared" si="3"/>
+      <c r="S11" s="31">
+        <f t="shared" si="4"/>
         <v>7.5809906716919201E-2</v>
       </c>
-      <c r="T10" s="34">
-        <f t="shared" si="3"/>
+      <c r="T11" s="31">
+        <f t="shared" si="4"/>
         <v>8.3957907802655468E-2</v>
       </c>
-      <c r="U10" s="34">
-        <f t="shared" si="3"/>
+      <c r="U11" s="31">
+        <f t="shared" si="4"/>
         <v>9.0491155930220807E-2</v>
       </c>
-      <c r="V10" s="34">
-        <f t="shared" si="3"/>
+      <c r="V11" s="31">
+        <f t="shared" si="4"/>
         <v>8.7292911674379511E-2</v>
       </c>
-      <c r="W10" s="34">
-        <f t="shared" si="3"/>
+      <c r="W11" s="31">
+        <f t="shared" si="4"/>
         <v>8.4559476507209547E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11">
-        <v>1994</v>
-      </c>
-      <c r="C11">
-        <v>2135</v>
-      </c>
-      <c r="D11">
-        <v>2255</v>
-      </c>
-      <c r="E11">
-        <v>2452</v>
-      </c>
-      <c r="F11">
-        <v>2489</v>
-      </c>
-      <c r="G11">
-        <v>2479</v>
-      </c>
-      <c r="H11">
-        <v>2695</v>
-      </c>
-      <c r="I11">
-        <v>2859</v>
-      </c>
-      <c r="J11">
-        <v>2991</v>
-      </c>
-      <c r="K11">
-        <v>3143</v>
-      </c>
-      <c r="L11">
-        <v>3326</v>
-      </c>
-      <c r="M11">
-        <v>3565</v>
-      </c>
-      <c r="N11">
-        <v>3815</v>
-      </c>
-      <c r="O11">
-        <v>4093</v>
-      </c>
-      <c r="P11">
-        <v>4378</v>
-      </c>
-      <c r="Q11">
-        <v>4560</v>
-      </c>
-      <c r="R11">
-        <v>1779</v>
-      </c>
-      <c r="S11">
-        <v>2304</v>
-      </c>
-      <c r="T11">
-        <v>3452</v>
-      </c>
-      <c r="U11">
-        <v>4426</v>
-      </c>
-      <c r="V11">
-        <v>4779</v>
-      </c>
-      <c r="W11" s="23">
-        <v>4988</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12">
-        <v>40.9</v>
+        <v>1994</v>
       </c>
       <c r="C12">
-        <v>41.9</v>
+        <v>2135</v>
       </c>
       <c r="D12">
-        <v>44.6</v>
+        <v>2255</v>
       </c>
       <c r="E12">
-        <v>46.7</v>
+        <v>2452</v>
       </c>
       <c r="F12">
-        <v>46.4</v>
+        <v>2489</v>
       </c>
       <c r="G12">
-        <v>42.3</v>
+        <v>2479</v>
       </c>
       <c r="H12">
-        <v>50.5</v>
+        <v>2695</v>
       </c>
       <c r="I12">
-        <v>50.7</v>
+        <v>2859</v>
       </c>
       <c r="J12">
-        <v>50.7</v>
+        <v>2991</v>
       </c>
       <c r="K12">
-        <v>51.7</v>
+        <v>3143</v>
       </c>
       <c r="L12">
-        <v>54</v>
+        <v>3326</v>
       </c>
       <c r="M12">
-        <v>54.8</v>
+        <v>3565</v>
       </c>
       <c r="N12">
-        <v>57</v>
+        <v>3815</v>
       </c>
       <c r="O12">
-        <v>61.5</v>
+        <v>4093</v>
       </c>
       <c r="P12">
-        <v>63.3</v>
-      </c>
-      <c r="W12" s="23"/>
+        <v>4378</v>
+      </c>
+      <c r="Q12">
+        <v>4560</v>
+      </c>
+      <c r="R12">
+        <v>1779</v>
+      </c>
+      <c r="S12">
+        <v>2304</v>
+      </c>
+      <c r="T12">
+        <v>3452</v>
+      </c>
+      <c r="U12">
+        <v>4426</v>
+      </c>
+      <c r="V12">
+        <v>4779</v>
+      </c>
+      <c r="W12" s="23">
+        <v>4988</v>
+      </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13">
+        <v>40.9</v>
+      </c>
+      <c r="C13">
+        <v>41.9</v>
+      </c>
+      <c r="D13">
+        <v>44.6</v>
+      </c>
+      <c r="E13">
+        <v>46.7</v>
+      </c>
+      <c r="F13">
+        <v>46.4</v>
+      </c>
+      <c r="G13">
+        <v>42.3</v>
+      </c>
+      <c r="H13">
+        <v>50.5</v>
+      </c>
+      <c r="I13">
+        <v>50.7</v>
+      </c>
+      <c r="J13">
+        <v>50.7</v>
+      </c>
+      <c r="K13">
+        <v>51.7</v>
+      </c>
+      <c r="L13">
         <v>54</v>
       </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>3.5</v>
-      </c>
-      <c r="D13">
-        <v>4</v>
-      </c>
-      <c r="E13">
-        <v>4</v>
-      </c>
-      <c r="F13">
-        <v>1.5</v>
-      </c>
-      <c r="G13">
-        <v>-2</v>
-      </c>
-      <c r="H13">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="I13">
-        <v>2.5</v>
-      </c>
-      <c r="J13">
-        <v>2.5</v>
-      </c>
-      <c r="K13">
-        <v>2.7</v>
-      </c>
-      <c r="L13">
-        <v>2.7</v>
-      </c>
       <c r="M13">
-        <v>3.2</v>
+        <v>54.8</v>
       </c>
       <c r="N13">
-        <v>3.4</v>
+        <v>57</v>
       </c>
       <c r="O13">
-        <v>3.4</v>
+        <v>61.5</v>
       </c>
       <c r="P13">
-        <v>3.1</v>
-      </c>
-      <c r="Q13">
-        <v>2.9</v>
-      </c>
-      <c r="R13">
-        <v>-2.7</v>
-      </c>
-      <c r="S13">
-        <v>6.6</v>
-      </c>
-      <c r="T13">
-        <v>3.6</v>
-      </c>
-      <c r="U13">
-        <v>3.5</v>
-      </c>
-      <c r="V13">
-        <v>3.3</v>
-      </c>
-      <c r="W13" s="23">
-        <v>2.5</v>
-      </c>
+        <v>63.3</v>
+      </c>
+      <c r="W13" s="23"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>3.5</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <v>1.5</v>
+      </c>
+      <c r="G14">
+        <v>-2</v>
+      </c>
+      <c r="H14">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I14">
+        <v>2.5</v>
+      </c>
+      <c r="J14">
+        <v>2.5</v>
+      </c>
+      <c r="K14">
+        <v>2.7</v>
+      </c>
+      <c r="L14">
+        <v>2.7</v>
+      </c>
+      <c r="M14">
+        <v>3.2</v>
+      </c>
+      <c r="N14">
+        <v>3.4</v>
+      </c>
+      <c r="O14">
+        <v>3.4</v>
+      </c>
+      <c r="P14">
+        <v>3.1</v>
+      </c>
+      <c r="Q14">
+        <v>2.9</v>
+      </c>
+      <c r="R14">
+        <v>-2.7</v>
+      </c>
+      <c r="S14">
+        <v>6.6</v>
+      </c>
+      <c r="T14">
+        <v>3.6</v>
+      </c>
+      <c r="U14">
+        <v>3.5</v>
+      </c>
+      <c r="V14">
+        <v>3.3</v>
+      </c>
+      <c r="W14" s="23">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>376</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>409</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>450</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <v>490</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>571</v>
       </c>
-      <c r="G14">
+      <c r="G15">
         <v>474</v>
       </c>
-      <c r="H14">
+      <c r="H15">
         <v>536</v>
       </c>
-      <c r="I14">
+      <c r="I15">
         <v>623</v>
       </c>
-      <c r="J14">
+      <c r="J15">
         <v>687</v>
       </c>
-      <c r="K14">
+      <c r="K15">
         <v>695</v>
       </c>
-      <c r="L14">
+      <c r="L15">
         <v>731</v>
       </c>
-      <c r="M14">
+      <c r="M15">
         <v>659</v>
       </c>
-      <c r="N14">
+      <c r="N15">
         <v>649</v>
       </c>
-      <c r="O14">
+      <c r="O15">
         <v>697</v>
       </c>
-      <c r="P14">
+      <c r="P15">
         <v>766</v>
       </c>
-      <c r="Q14">
+      <c r="Q15">
         <v>795</v>
       </c>
-      <c r="R14">
+      <c r="R15">
         <v>495</v>
       </c>
-      <c r="S14">
+      <c r="S15">
         <v>556</v>
       </c>
-      <c r="T14">
+      <c r="T15">
         <v>727</v>
       </c>
-      <c r="U14">
+      <c r="U15">
         <v>846</v>
       </c>
-      <c r="V14">
+      <c r="V15">
         <v>904</v>
       </c>
-      <c r="W14" s="23">
+      <c r="W15" s="23">
         <v>913</v>
       </c>
     </row>
-    <row r="15" spans="1:23" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="33" t="s">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="31">
+        <f>(B4/(B2+B4))*B15</f>
+        <v>56.26923939869868</v>
+      </c>
+      <c r="C16" s="31">
+        <f t="shared" ref="C16:W16" si="5">(C4/(C2+C4))*C15</f>
+        <v>58.258720930232549</v>
+      </c>
+      <c r="D16" s="31">
+        <f t="shared" si="5"/>
+        <v>63.359201773835913</v>
+      </c>
+      <c r="E16" s="31">
+        <f t="shared" si="5"/>
+        <v>69.363743477529027</v>
+      </c>
+      <c r="F16" s="31">
+        <f t="shared" si="5"/>
+        <v>76.289557683538533</v>
+      </c>
+      <c r="G16" s="31">
+        <f t="shared" si="5"/>
+        <v>61.222832052689341</v>
+      </c>
+      <c r="H16" s="31">
+        <f t="shared" si="5"/>
+        <v>72.769843702114613</v>
+      </c>
+      <c r="I16" s="31">
+        <f t="shared" si="5"/>
+        <v>81.114076683376226</v>
+      </c>
+      <c r="J16" s="31">
+        <f t="shared" si="5"/>
+        <v>81.55498689302209</v>
+      </c>
+      <c r="K16" s="31">
+        <f t="shared" si="5"/>
+        <v>78.819726634650891</v>
+      </c>
+      <c r="L16" s="31">
+        <f t="shared" si="5"/>
+        <v>78.974183044540069</v>
+      </c>
+      <c r="M16" s="31">
+        <f t="shared" si="5"/>
+        <v>68.61853876739562</v>
+      </c>
+      <c r="N16" s="31">
+        <f t="shared" si="5"/>
+        <v>66.395543175487475</v>
+      </c>
+      <c r="O16" s="31">
+        <f t="shared" si="5"/>
+        <v>78.647252617955061</v>
+      </c>
+      <c r="P16" s="31">
+        <f t="shared" si="5"/>
+        <v>92.338134950720246</v>
+      </c>
+      <c r="Q16" s="31">
+        <f t="shared" si="5"/>
+        <v>85.511182108626201</v>
+      </c>
+      <c r="R16" s="31">
+        <f t="shared" si="5"/>
+        <v>132.25190839694656</v>
+      </c>
+      <c r="S16" s="31">
+        <f t="shared" si="5"/>
+        <v>161.49377593360998</v>
+      </c>
+      <c r="T16" s="31">
+        <f t="shared" si="5"/>
+        <v>158.64618644067798</v>
+      </c>
+      <c r="U16" s="31">
+        <f t="shared" si="5"/>
+        <v>112.20801526717558</v>
+      </c>
+      <c r="V16" s="31">
+        <f t="shared" si="5"/>
+        <v>120.80358744394618</v>
+      </c>
+      <c r="W16" s="31">
+        <f t="shared" si="5"/>
+        <v>115.6520963425513</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="34">
-        <f>(B3/(B3+B4))*B14</f>
+      <c r="B17" s="31">
+        <f>(B3/(B3+B4))*B15</f>
         <v>306.47075131688388</v>
       </c>
-      <c r="C15" s="34">
-        <f t="shared" ref="C15:W15" si="4">(C3/(C3+C4))*C14</f>
+      <c r="C17" s="31">
+        <f t="shared" ref="C17:W17" si="6">(C3/(C3+C4))*C15</f>
         <v>337.35188968335035</v>
       </c>
-      <c r="D15" s="34">
-        <f t="shared" si="4"/>
+      <c r="D17" s="31">
+        <f t="shared" si="6"/>
         <v>372.2801450589302</v>
       </c>
-      <c r="E15" s="34">
-        <f t="shared" si="4"/>
+      <c r="E17" s="31">
+        <f t="shared" si="6"/>
         <v>404.69882012005792</v>
       </c>
-      <c r="F15" s="34">
-        <f t="shared" si="4"/>
+      <c r="F17" s="31">
+        <f t="shared" si="6"/>
         <v>476.63846587704461</v>
       </c>
-      <c r="G15" s="34">
-        <f t="shared" si="4"/>
+      <c r="G17" s="31">
+        <f t="shared" si="6"/>
         <v>398.73144399460188</v>
       </c>
-      <c r="H15" s="34">
-        <f t="shared" si="4"/>
+      <c r="H17" s="31">
+        <f t="shared" si="6"/>
         <v>447.00149925037482</v>
       </c>
-      <c r="I15" s="34">
-        <f t="shared" si="4"/>
+      <c r="I17" s="31">
+        <f t="shared" si="6"/>
         <v>524.05718063130064</v>
       </c>
-      <c r="J15" s="34">
-        <f t="shared" si="4"/>
+      <c r="J17" s="31">
+        <f t="shared" si="6"/>
         <v>582.14732787674529</v>
       </c>
-      <c r="K15" s="34">
-        <f t="shared" si="4"/>
+      <c r="K17" s="31">
+        <f t="shared" si="6"/>
         <v>593.25226514067708</v>
       </c>
-      <c r="L15" s="34">
-        <f t="shared" si="4"/>
+      <c r="L17" s="31">
+        <f t="shared" si="6"/>
         <v>623.18939514208603</v>
       </c>
-      <c r="M15" s="34">
-        <f t="shared" si="4"/>
+      <c r="M17" s="31">
+        <f t="shared" si="6"/>
         <v>570.18655516243166</v>
       </c>
-      <c r="N15" s="34">
-        <f t="shared" si="4"/>
+      <c r="N17" s="31">
+        <f t="shared" si="6"/>
         <v>560.08986096982039</v>
       </c>
-      <c r="O15" s="34">
-        <f t="shared" si="4"/>
+      <c r="O17" s="31">
+        <f t="shared" si="6"/>
         <v>590.88426734402287</v>
       </c>
-      <c r="P15" s="34">
-        <f t="shared" si="4"/>
+      <c r="P17" s="31">
+        <f t="shared" si="6"/>
         <v>639.1878625613565</v>
       </c>
-      <c r="Q15" s="34">
-        <f t="shared" si="4"/>
+      <c r="Q17" s="31">
+        <f t="shared" si="6"/>
         <v>681.58898305084745</v>
       </c>
-      <c r="R15" s="34">
-        <f t="shared" si="4"/>
+      <c r="R17" s="31">
+        <f t="shared" si="6"/>
         <v>284.36170212765961</v>
       </c>
-      <c r="S15" s="34">
-        <f t="shared" si="4"/>
+      <c r="S17" s="31">
+        <f t="shared" si="6"/>
         <v>297.68141592920358</v>
       </c>
-      <c r="T15" s="34">
-        <f t="shared" si="4"/>
+      <c r="T17" s="31">
+        <f t="shared" si="6"/>
         <v>494.08864696734059</v>
       </c>
-      <c r="U15" s="34">
-        <f t="shared" si="4"/>
+      <c r="U17" s="31">
+        <f t="shared" si="6"/>
         <v>696.57941550190594</v>
       </c>
-      <c r="V15" s="34">
-        <f t="shared" si="4"/>
+      <c r="V17" s="31">
+        <f t="shared" si="6"/>
         <v>741.91095066185312</v>
       </c>
-      <c r="W15" s="34">
-        <f t="shared" si="4"/>
+      <c r="W17" s="31">
+        <f t="shared" si="6"/>
         <v>757.73532934131731</v>
       </c>
     </row>
-    <row r="16" spans="1:23" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+    <row r="18" spans="1:23" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="34">
-        <f>B15/B6</f>
+      <c r="B18" s="31">
+        <f>B17/B7</f>
         <v>8.4925292228215585E-2</v>
       </c>
-      <c r="C16" s="34">
-        <f t="shared" ref="C16:W16" si="5">C15/C6</f>
+      <c r="C18" s="31">
+        <f t="shared" ref="C18:W18" si="7">C17/C7</f>
         <v>8.6199669789107841E-2</v>
       </c>
-      <c r="D16" s="34">
-        <f t="shared" si="5"/>
+      <c r="D18" s="31">
+        <f t="shared" si="7"/>
         <v>8.9387280315724696E-2</v>
       </c>
-      <c r="E16" s="34">
-        <f t="shared" si="5"/>
+      <c r="E18" s="31">
+        <f t="shared" si="7"/>
         <v>8.9672025906817457E-2</v>
       </c>
-      <c r="F16" s="34">
-        <f t="shared" si="5"/>
+      <c r="F18" s="31">
+        <f t="shared" si="7"/>
         <v>0.10342661791810397</v>
       </c>
-      <c r="G16" s="34">
-        <f t="shared" si="5"/>
+      <c r="G18" s="31">
+        <f t="shared" si="7"/>
         <v>8.741407678647653E-2</v>
       </c>
-      <c r="H16" s="34">
-        <f t="shared" si="5"/>
+      <c r="H18" s="31">
+        <f t="shared" si="7"/>
         <v>9.0665077683763459E-2</v>
       </c>
-      <c r="I16" s="34">
-        <f t="shared" si="5"/>
+      <c r="I18" s="31">
+        <f t="shared" si="7"/>
         <v>9.9733789438373646E-2</v>
       </c>
-      <c r="J16" s="34">
-        <f t="shared" si="5"/>
+      <c r="J18" s="31">
+        <f t="shared" si="7"/>
         <v>0.10516350916547053</v>
       </c>
-      <c r="K16" s="34">
-        <f t="shared" si="5"/>
+      <c r="K18" s="31">
+        <f t="shared" si="7"/>
         <v>0.10158951061538728</v>
       </c>
-      <c r="L16" s="34">
-        <f t="shared" si="5"/>
+      <c r="L18" s="31">
+        <f t="shared" si="7"/>
         <v>0.10069729785741299</v>
       </c>
-      <c r="M16" s="34">
-        <f t="shared" si="5"/>
+      <c r="M18" s="31">
+        <f t="shared" si="7"/>
         <v>8.570638110663821E-2</v>
       </c>
-      <c r="N16" s="34">
-        <f t="shared" si="5"/>
+      <c r="N18" s="31">
+        <f t="shared" si="7"/>
         <v>7.8394549789323309E-2</v>
       </c>
-      <c r="O16" s="34">
-        <f t="shared" si="5"/>
+      <c r="O18" s="31">
+        <f t="shared" si="7"/>
         <v>7.6573732183598198E-2</v>
       </c>
-      <c r="P16" s="34">
-        <f t="shared" si="5"/>
+      <c r="P18" s="31">
+        <f t="shared" si="7"/>
         <v>7.7207977813319895E-2</v>
       </c>
-      <c r="Q16" s="34">
-        <f t="shared" si="5"/>
+      <c r="Q18" s="31">
+        <f t="shared" si="7"/>
         <v>7.8451770608983368E-2</v>
       </c>
-      <c r="R16" s="34">
-        <f t="shared" si="5"/>
+      <c r="R18" s="31">
+        <f t="shared" si="7"/>
         <v>9.5615905221136388E-2</v>
       </c>
-      <c r="S16" s="34">
-        <f t="shared" si="5"/>
+      <c r="S18" s="31">
+        <f t="shared" si="7"/>
         <v>8.2164343342313984E-2</v>
       </c>
-      <c r="T16" s="34">
-        <f t="shared" si="5"/>
+      <c r="T18" s="31">
+        <f t="shared" si="7"/>
         <v>8.270650267280559E-2</v>
       </c>
-      <c r="U16" s="34">
-        <f t="shared" si="5"/>
+      <c r="U18" s="31">
+        <f t="shared" si="7"/>
         <v>8.4219491657829271E-2</v>
       </c>
-      <c r="V16" s="34">
-        <f t="shared" si="5"/>
+      <c r="V18" s="31">
+        <f t="shared" si="7"/>
         <v>8.1690261028611877E-2</v>
       </c>
-      <c r="W16" s="34">
-        <f t="shared" si="5"/>
+      <c r="W18" s="31">
+        <f t="shared" si="7"/>
         <v>7.8858837641554977E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A17" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17">
-        <v>65</v>
-      </c>
-      <c r="C17">
-        <v>91</v>
-      </c>
-      <c r="D17">
-        <v>127</v>
-      </c>
-      <c r="E17">
-        <v>146</v>
-      </c>
-      <c r="F17">
-        <v>203</v>
-      </c>
-      <c r="G17">
-        <v>134</v>
-      </c>
-      <c r="H17">
-        <v>151</v>
-      </c>
-      <c r="I17">
-        <v>191</v>
-      </c>
-      <c r="J17">
-        <v>228</v>
-      </c>
-      <c r="K17">
-        <v>230</v>
-      </c>
-      <c r="L17">
-        <v>224</v>
-      </c>
-      <c r="M17">
-        <v>174</v>
-      </c>
-      <c r="N17">
-        <v>135</v>
-      </c>
-      <c r="O17">
-        <v>149</v>
-      </c>
-      <c r="P17">
-        <v>180</v>
-      </c>
-      <c r="Q17">
-        <v>190</v>
-      </c>
-      <c r="R17">
-        <v>80</v>
-      </c>
-      <c r="S17">
-        <v>106</v>
-      </c>
-      <c r="T17">
-        <v>215</v>
-      </c>
-      <c r="U17">
-        <v>269</v>
-      </c>
-      <c r="V17">
-        <v>261</v>
-      </c>
-      <c r="W17" s="23">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A18" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18">
-        <v>49.7</v>
-      </c>
-      <c r="C18">
-        <v>71</v>
-      </c>
-      <c r="D18">
-        <v>81.900000000000006</v>
-      </c>
-      <c r="E18">
-        <v>90</v>
-      </c>
-      <c r="F18">
-        <v>126.7</v>
-      </c>
-      <c r="G18">
-        <v>91.4</v>
-      </c>
-      <c r="H18">
-        <v>112.7</v>
-      </c>
-      <c r="I18">
-        <v>129.6</v>
-      </c>
-      <c r="J18">
-        <v>124.5</v>
-      </c>
-      <c r="K18">
-        <v>114.8</v>
-      </c>
-      <c r="L18">
-        <v>99.9</v>
-      </c>
-      <c r="M18">
-        <v>66.7</v>
-      </c>
-      <c r="N18">
-        <v>52.1</v>
-      </c>
-      <c r="O18">
-        <v>66.7</v>
-      </c>
-      <c r="P18">
-        <v>86.1</v>
-      </c>
-      <c r="Q18">
-        <v>80</v>
-      </c>
-      <c r="R18">
-        <v>47</v>
-      </c>
-      <c r="S18">
-        <v>78</v>
-      </c>
-      <c r="T18">
-        <v>139</v>
-      </c>
-      <c r="U18">
-        <v>112</v>
-      </c>
-      <c r="V18">
-        <v>99</v>
-      </c>
-      <c r="W18" s="23">
-        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B19">
-        <v>311</v>
+        <v>65</v>
       </c>
       <c r="C19">
-        <v>318</v>
+        <v>91</v>
       </c>
       <c r="D19">
-        <v>324</v>
+        <v>127</v>
       </c>
       <c r="E19">
-        <v>344</v>
+        <v>146</v>
       </c>
       <c r="F19">
-        <v>367</v>
+        <v>203</v>
       </c>
       <c r="G19">
-        <v>340</v>
+        <v>134</v>
       </c>
       <c r="H19">
-        <v>385</v>
+        <v>151</v>
       </c>
       <c r="I19">
-        <v>431</v>
+        <v>191</v>
       </c>
       <c r="J19">
-        <v>459</v>
+        <v>228</v>
       </c>
       <c r="K19">
-        <v>464</v>
+        <v>230</v>
       </c>
       <c r="L19">
-        <v>507</v>
+        <v>224</v>
       </c>
       <c r="M19">
-        <v>485</v>
+        <v>174</v>
       </c>
       <c r="N19">
-        <v>514</v>
+        <v>135</v>
       </c>
       <c r="O19">
-        <v>548</v>
+        <v>149</v>
       </c>
       <c r="P19">
-        <v>586</v>
+        <v>180</v>
       </c>
       <c r="Q19">
-        <v>605</v>
+        <v>190</v>
       </c>
       <c r="R19">
-        <v>415</v>
+        <v>80</v>
       </c>
       <c r="S19">
-        <v>450</v>
+        <v>106</v>
       </c>
       <c r="T19">
-        <v>512</v>
+        <v>215</v>
       </c>
       <c r="U19">
-        <v>577</v>
+        <v>269</v>
       </c>
       <c r="V19">
-        <v>643</v>
+        <v>261</v>
       </c>
       <c r="W19" s="23">
-        <v>677</v>
+        <v>236</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B20">
-        <v>3.3</v>
+        <v>49.7</v>
       </c>
       <c r="C20">
-        <v>4.4000000000000004</v>
+        <v>71</v>
       </c>
       <c r="D20">
-        <v>15</v>
+        <v>81.900000000000006</v>
       </c>
       <c r="E20">
-        <v>19.899999999999999</v>
+        <v>90</v>
       </c>
       <c r="F20">
-        <v>-1.1000000000000001</v>
+        <v>126.7</v>
       </c>
       <c r="G20">
-        <v>1.9</v>
+        <v>91.4</v>
       </c>
       <c r="H20">
-        <v>27.6</v>
+        <v>112.7</v>
       </c>
       <c r="I20">
-        <v>19.8</v>
+        <v>129.6</v>
       </c>
       <c r="J20">
-        <v>18.399999999999999</v>
+        <v>124.5</v>
       </c>
       <c r="K20">
-        <v>25.3</v>
+        <v>114.8</v>
       </c>
       <c r="L20">
-        <v>35.5</v>
+        <v>99.9</v>
       </c>
       <c r="M20">
-        <v>62</v>
+        <v>66.7</v>
       </c>
       <c r="N20">
-        <v>60.1</v>
+        <v>52.1</v>
       </c>
       <c r="O20">
-        <v>56.3</v>
+        <v>66.7</v>
       </c>
       <c r="P20">
-        <v>45.9</v>
+        <v>86.1</v>
       </c>
       <c r="Q20">
-        <v>43.1</v>
+        <v>80</v>
       </c>
       <c r="R20">
-        <v>-110.9</v>
+        <v>47</v>
       </c>
       <c r="S20">
-        <v>-43.5</v>
+        <v>78</v>
       </c>
       <c r="T20">
-        <v>11.3</v>
+        <v>139</v>
       </c>
       <c r="U20">
-        <v>62.9</v>
+        <v>112</v>
       </c>
       <c r="V20">
-        <v>61.9</v>
+        <v>99</v>
       </c>
       <c r="W20" s="23">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B21">
-        <v>0.9</v>
+        <v>311</v>
       </c>
       <c r="C21">
-        <v>1.1000000000000001</v>
+        <v>318</v>
       </c>
       <c r="D21">
-        <v>3.2</v>
+        <v>324</v>
       </c>
       <c r="E21">
-        <v>3.9</v>
+        <v>344</v>
       </c>
       <c r="F21">
-        <v>-0.2</v>
+        <v>367</v>
       </c>
       <c r="G21">
-        <v>0.4</v>
+        <v>340</v>
       </c>
       <c r="H21">
-        <v>4.9000000000000004</v>
+        <v>385</v>
       </c>
       <c r="I21">
-        <v>3.1</v>
+        <v>431</v>
       </c>
       <c r="J21">
-        <v>2.6</v>
+        <v>459</v>
       </c>
       <c r="K21">
-        <v>3.5</v>
+        <v>464</v>
       </c>
       <c r="L21">
-        <v>4.5999999999999996</v>
+        <v>507</v>
       </c>
       <c r="M21">
-        <v>8.6</v>
+        <v>485</v>
       </c>
       <c r="N21">
-        <v>8.5</v>
+        <v>514</v>
       </c>
       <c r="O21">
-        <v>7.5</v>
+        <v>548</v>
       </c>
       <c r="P21">
-        <v>5.7</v>
+        <v>586</v>
       </c>
       <c r="Q21">
-        <v>5.0999999999999996</v>
+        <v>605</v>
       </c>
       <c r="R21">
-        <v>-28.8</v>
+        <v>415</v>
       </c>
       <c r="S21">
-        <v>-8.5</v>
+        <v>450</v>
       </c>
       <c r="T21">
-        <v>1.5</v>
+        <v>512</v>
       </c>
       <c r="U21">
-        <v>6.9</v>
+        <v>577</v>
       </c>
       <c r="V21">
-        <v>6.4</v>
+        <v>643</v>
       </c>
       <c r="W21" s="23">
-        <v>6.7</v>
+        <v>677</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22">
+        <v>3.3</v>
+      </c>
+      <c r="C22">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D22">
+        <v>15</v>
+      </c>
+      <c r="E22">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="F22">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="G22">
+        <v>1.9</v>
+      </c>
+      <c r="H22">
+        <v>27.6</v>
+      </c>
+      <c r="I22">
+        <v>19.8</v>
+      </c>
+      <c r="J22">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="K22">
+        <v>25.3</v>
+      </c>
+      <c r="L22">
+        <v>35.5</v>
+      </c>
+      <c r="M22">
+        <v>62</v>
+      </c>
+      <c r="N22">
+        <v>60.1</v>
+      </c>
+      <c r="O22">
+        <v>56.3</v>
+      </c>
+      <c r="P22">
+        <v>45.9</v>
+      </c>
+      <c r="Q22">
+        <v>43.1</v>
+      </c>
+      <c r="R22">
+        <v>-110.9</v>
+      </c>
+      <c r="S22">
+        <v>-43.5</v>
+      </c>
+      <c r="T22">
+        <v>11.3</v>
+      </c>
+      <c r="U22">
+        <v>62.9</v>
+      </c>
+      <c r="V22">
+        <v>61.9</v>
+      </c>
+      <c r="W22" s="23">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A23" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23">
+        <v>0.9</v>
+      </c>
+      <c r="C23">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D23">
+        <v>3.2</v>
+      </c>
+      <c r="E23">
+        <v>3.9</v>
+      </c>
+      <c r="F23">
+        <v>-0.2</v>
+      </c>
+      <c r="G23">
+        <v>0.4</v>
+      </c>
+      <c r="H23">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I23">
+        <v>3.1</v>
+      </c>
+      <c r="J23">
+        <v>2.6</v>
+      </c>
+      <c r="K23">
+        <v>3.5</v>
+      </c>
+      <c r="L23">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="M23">
+        <v>8.6</v>
+      </c>
+      <c r="N23">
+        <v>8.5</v>
+      </c>
+      <c r="O23">
+        <v>7.5</v>
+      </c>
+      <c r="P23">
+        <v>5.7</v>
+      </c>
+      <c r="Q23">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="R23">
+        <v>-28.8</v>
+      </c>
+      <c r="S23">
+        <v>-8.5</v>
+      </c>
+      <c r="T23">
+        <v>1.5</v>
+      </c>
+      <c r="U23">
+        <v>6.9</v>
+      </c>
+      <c r="V23">
+        <v>6.4</v>
+      </c>
+      <c r="W23" s="23">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A24" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B22">
+      <c r="B24">
         <v>-5.6</v>
       </c>
-      <c r="C22">
+      <c r="C24">
         <v>-4.0999999999999996</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <v>5</v>
       </c>
-      <c r="E22">
+      <c r="E24">
         <v>14.7</v>
       </c>
-      <c r="F22">
+      <c r="F24">
         <v>-26.1</v>
       </c>
-      <c r="G22">
+      <c r="G24">
         <v>-4.5999999999999996</v>
       </c>
-      <c r="H22">
+      <c r="H24">
         <v>17.3</v>
       </c>
-      <c r="I22">
+      <c r="I24">
         <v>8.3000000000000007</v>
       </c>
-      <c r="J22">
+      <c r="J24">
         <v>9.1999999999999993</v>
       </c>
-      <c r="K22">
+      <c r="K24">
         <v>10.7</v>
       </c>
-      <c r="L22">
+      <c r="L24">
         <v>13.8</v>
       </c>
-      <c r="M22">
+      <c r="M24">
         <v>36</v>
       </c>
-      <c r="N22">
+      <c r="N24">
         <v>34.200000000000003</v>
       </c>
-      <c r="O22">
+      <c r="O24">
         <v>38</v>
       </c>
-      <c r="P22">
+      <c r="P24">
         <v>27.3</v>
       </c>
-      <c r="Q22">
+      <c r="Q24">
         <v>26.4</v>
       </c>
-      <c r="R22">
+      <c r="R24">
         <v>-138.69999999999999</v>
       </c>
-      <c r="S22">
+      <c r="S24">
         <v>-40.4</v>
       </c>
-      <c r="T22">
+      <c r="T24">
         <v>-3.5</v>
       </c>
-      <c r="U22">
+      <c r="U24">
         <v>37.299999999999997</v>
       </c>
-      <c r="V22">
+      <c r="V24">
         <v>32.4</v>
       </c>
-      <c r="W22" s="23">
+      <c r="W24" s="23">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A23" s="29" t="s">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A25" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="25">
+      <c r="B25" s="25">
         <v>-1.5</v>
       </c>
-      <c r="C23" s="25">
+      <c r="C25" s="25">
         <v>-1</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D25" s="25">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E25" s="25">
         <v>2.9</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F25" s="25">
         <v>-4.5999999999999996</v>
       </c>
-      <c r="G23" s="25">
+      <c r="G25" s="25">
         <v>-1</v>
       </c>
-      <c r="H23" s="25">
+      <c r="H25" s="25">
         <v>3.1</v>
       </c>
-      <c r="I23" s="25">
+      <c r="I25" s="25">
         <v>1.3</v>
       </c>
-      <c r="J23" s="25">
+      <c r="J25" s="25">
         <v>1.3</v>
       </c>
-      <c r="K23" s="25">
+      <c r="K25" s="25">
         <v>1.5</v>
       </c>
-      <c r="L23" s="25">
+      <c r="L25" s="25">
         <v>1.8</v>
       </c>
-      <c r="M23" s="25">
+      <c r="M25" s="25">
         <v>5</v>
       </c>
-      <c r="N23" s="25">
+      <c r="N25" s="25">
         <v>4.8</v>
       </c>
-      <c r="O23" s="25">
+      <c r="O25" s="25">
         <v>5</v>
       </c>
-      <c r="P23" s="25">
+      <c r="P25" s="25">
         <v>4.0999999999999996</v>
       </c>
-      <c r="Q23" s="25">
+      <c r="Q25" s="25">
         <v>3.1</v>
       </c>
-      <c r="R23" s="25">
+      <c r="R25" s="25">
         <v>-35.799999999999997</v>
       </c>
-      <c r="S23" s="25">
+      <c r="S25" s="25">
         <v>-7.9</v>
       </c>
-      <c r="T23" s="25">
+      <c r="T25" s="25">
         <v>-0.5</v>
       </c>
-      <c r="U23" s="25">
+      <c r="U25" s="25">
         <v>4.0999999999999996</v>
       </c>
-      <c r="V23" s="25">
+      <c r="V25" s="25">
         <v>3.4</v>
       </c>
-      <c r="W23" s="26">
+      <c r="W25" s="26">
         <v>3.7</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="V24" t="s">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="V26" t="s">
         <v>70</v>
       </c>
-      <c r="W24" t="s">
+      <c r="W26" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>61</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B60" t="s">
         <v>64</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C60" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
-        <v>65</v>
-      </c>
-      <c r="C59" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B60" t="s">
-        <v>66</v>
-      </c>
-      <c r="C60" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
         <v>68</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C63" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>